<commit_message>
Se realiza la estimacion de tiempo en el documento Asignacion de recursos y tiempo
</commit_message>
<xml_diff>
--- a/Proyecto/Tercer Incremento - Segunda Entrega/Documentos/(SnoutPoint) - Asignación de Recursos y Tiempo.xlsx
+++ b/Proyecto/Tercer Incremento - Segunda Entrega/Documentos/(SnoutPoint) - Asignación de Recursos y Tiempo.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="20730" windowHeight="9555" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="48" windowWidth="20736" windowHeight="9552" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1° Inc - Recursos y Costos" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="4° - Recursos y Costos" sheetId="4" r:id="rId4"/>
     <sheet name="5° - Recursos y Costos" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -216,7 +216,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="172">
   <si>
     <t>Id</t>
   </si>
@@ -739,11 +739,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
-    <numFmt numFmtId="165" formatCode="_-[$$-240A]\ * #,##0.00_ ;_-[$$-240A]\ * \-#,##0.00\ ;_-[$$-240A]\ * &quot;-&quot;??_ ;_-@_ "/>
-    <numFmt numFmtId="166" formatCode="[$-C0A]d\-mmm\-yyyy;@"/>
-    <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="_-[$$-240A]\ * #,##0.00_ ;_-[$$-240A]\ * \-#,##0.00\ ;_-[$$-240A]\ * &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="167" formatCode="[$-C0A]d\-mmm\-yyyy;@"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -1259,8 +1259,8 @@
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="225">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1321,7 +1321,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1333,13 +1333,13 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1369,43 +1369,43 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="8" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="6" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="8" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="6" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="10" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="10" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1417,10 +1417,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1435,7 +1435,7 @@
     <xf numFmtId="0" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1447,7 +1447,7 @@
     <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="8" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="10" fillId="8" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1465,10 +1465,10 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1486,7 +1486,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1531,7 +1531,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1543,7 +1543,7 @@
     <xf numFmtId="14" fontId="11" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="10" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1561,13 +1561,13 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1594,17 +1594,17 @@
     <xf numFmtId="14" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1622,7 +1622,7 @@
     <xf numFmtId="14" fontId="11" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="9" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="10" fillId="9" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1643,7 +1643,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="10" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1652,10 +1652,10 @@
     <xf numFmtId="0" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1685,10 +1685,10 @@
     <xf numFmtId="0" fontId="13" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="8" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="12" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="8" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1709,13 +1709,13 @@
     <xf numFmtId="14" fontId="13" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="9" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="12" fillId="9" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1727,7 +1727,7 @@
     <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1751,19 +1751,19 @@
     <xf numFmtId="0" fontId="13" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="12" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="12" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1784,16 +1784,16 @@
     <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="12" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1809,16 +1809,16 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="13" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="13" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1830,13 +1830,13 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="13" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="13" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1845,7 +1845,7 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1854,10 +1854,10 @@
     <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1887,18 +1887,21 @@
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1906,9 +1909,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2250,51 +2250,51 @@
   <dimension ref="A1:R68"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="K63" sqref="K63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="16" style="1" customWidth="1"/>
-    <col min="8" max="9" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="18.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="29" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.42578125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="62.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.44140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="62.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="31" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="11.5703125" style="1"/>
+    <col min="19" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="214" t="s">
+    <row r="1" spans="1:18" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="215" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="215"/>
-      <c r="C1" s="215"/>
-      <c r="D1" s="215"/>
-      <c r="E1" s="215"/>
-      <c r="F1" s="215"/>
-      <c r="G1" s="215"/>
-      <c r="H1" s="215"/>
-      <c r="I1" s="215"/>
-      <c r="J1" s="215"/>
-      <c r="K1" s="215"/>
-      <c r="L1" s="216"/>
-    </row>
-    <row r="2" spans="1:18" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="216"/>
+      <c r="C1" s="216"/>
+      <c r="D1" s="216"/>
+      <c r="E1" s="216"/>
+      <c r="F1" s="216"/>
+      <c r="G1" s="216"/>
+      <c r="H1" s="216"/>
+      <c r="I1" s="216"/>
+      <c r="J1" s="216"/>
+      <c r="K1" s="216"/>
+      <c r="L1" s="217"/>
+    </row>
+    <row r="2" spans="1:18" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="83" t="s">
         <v>0</v>
       </c>
@@ -2389,7 +2389,7 @@
       <c r="Q3" s="6"/>
       <c r="R3" s="5"/>
     </row>
-    <row r="4" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="189">
         <v>2</v>
       </c>
@@ -2434,7 +2434,7 @@
       <c r="Q4" s="8"/>
       <c r="R4" s="7"/>
     </row>
-    <row r="5" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="32">
         <v>3</v>
       </c>
@@ -2479,7 +2479,7 @@
       <c r="Q5" s="10"/>
       <c r="R5" s="7"/>
     </row>
-    <row r="6" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="32">
         <v>4</v>
       </c>
@@ -2524,7 +2524,7 @@
       <c r="Q6" s="11"/>
       <c r="R6" s="12"/>
     </row>
-    <row r="7" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="32">
         <v>5</v>
       </c>
@@ -2563,7 +2563,7 @@
       <c r="Q7" s="13"/>
       <c r="R7" s="14"/>
     </row>
-    <row r="8" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="32">
         <v>6</v>
       </c>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="M8" s="44"/>
     </row>
-    <row r="9" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="32">
         <v>7</v>
       </c>
@@ -2638,7 +2638,7 @@
         <v>3528.6458333333335</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="32">
         <v>8</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>3528.6458333333335</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="32">
         <v>9</v>
       </c>
@@ -2712,7 +2712,7 @@
         <v>3528.6458333333335</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A12" s="32">
         <v>10</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>3528.6458333333335</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="32">
         <v>11</v>
       </c>
@@ -2786,7 +2786,7 @@
         <v>3528.6458333333335</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="32">
         <v>12</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>3528.6458333333335</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="32">
         <v>13</v>
       </c>
@@ -2860,7 +2860,7 @@
         <v>3528.6458333333335</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="32">
         <v>14</v>
       </c>
@@ -3136,7 +3136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11">
         <v>22</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>1764.3229166666667</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11">
         <v>23</v>
       </c>
@@ -3212,7 +3212,7 @@
         <v>7057.291666666667</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="22">
         <v>24</v>
       </c>
@@ -3302,7 +3302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="11">
         <v>27</v>
       </c>
@@ -3342,7 +3342,7 @@
         <v>3528.6458333333335</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11">
         <v>28</v>
       </c>
@@ -3378,7 +3378,7 @@
         <v>7057.291666666667</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11">
         <v>29</v>
       </c>
@@ -3412,7 +3412,7 @@
         <v>28229.166666666668</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11">
         <v>30</v>
       </c>
@@ -3446,7 +3446,7 @@
         <v>7057.291666666667</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="11">
         <v>31</v>
       </c>
@@ -3486,7 +3486,7 @@
         <v>3528.6458333333335</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="10">
         <v>32</v>
       </c>
@@ -3510,7 +3510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="11">
         <v>33</v>
       </c>
@@ -3542,7 +3542,7 @@
         <v>232890.625</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="22">
         <v>34</v>
       </c>
@@ -3582,7 +3582,7 @@
         <v>105859.375</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="22">
         <v>35</v>
       </c>
@@ -3622,7 +3622,7 @@
         <v>127031.25</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="11">
         <v>36</v>
       </c>
@@ -3660,7 +3660,7 @@
         <v>10585.9375</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="22">
         <v>37</v>
       </c>
@@ -3693,16 +3693,16 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O39" s="217" t="s">
+      <c r="O39" s="214" t="s">
         <v>115</v>
       </c>
-      <c r="P39" s="217"/>
-      <c r="Q39" s="217" t="s">
+      <c r="P39" s="214"/>
+      <c r="Q39" s="214" t="s">
         <v>116</v>
       </c>
-      <c r="R39" s="217"/>
-    </row>
-    <row r="40" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R39" s="214"/>
+    </row>
+    <row r="40" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="22">
         <v>38</v>
       </c>
@@ -3741,12 +3741,12 @@
       <c r="P40" s="46">
         <v>42042</v>
       </c>
-      <c r="Q40" s="217">
+      <c r="Q40" s="214">
         <v>1</v>
       </c>
-      <c r="R40" s="217"/>
-    </row>
-    <row r="41" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R40" s="214"/>
+    </row>
+    <row r="41" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="22">
         <v>39</v>
       </c>
@@ -3785,12 +3785,12 @@
       <c r="P41" s="46">
         <v>42049</v>
       </c>
-      <c r="Q41" s="217">
+      <c r="Q41" s="214">
         <v>2</v>
       </c>
-      <c r="R41" s="217"/>
-    </row>
-    <row r="42" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R41" s="214"/>
+    </row>
+    <row r="42" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="11">
         <v>40</v>
       </c>
@@ -3833,12 +3833,12 @@
       <c r="P42" s="46">
         <v>42056</v>
       </c>
-      <c r="Q42" s="217">
+      <c r="Q42" s="214">
         <v>3</v>
       </c>
-      <c r="R42" s="217"/>
-    </row>
-    <row r="43" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R42" s="214"/>
+    </row>
+    <row r="43" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="11">
         <v>41</v>
       </c>
@@ -3871,12 +3871,12 @@
       <c r="P43" s="46">
         <v>42063</v>
       </c>
-      <c r="Q43" s="217">
+      <c r="Q43" s="214">
         <v>4</v>
       </c>
-      <c r="R43" s="217"/>
-    </row>
-    <row r="44" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R43" s="214"/>
+    </row>
+    <row r="44" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="22">
         <v>42</v>
       </c>
@@ -3921,12 +3921,12 @@
       <c r="P44" s="46">
         <v>42070</v>
       </c>
-      <c r="Q44" s="217">
+      <c r="Q44" s="214">
         <v>5</v>
       </c>
-      <c r="R44" s="217"/>
-    </row>
-    <row r="45" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R44" s="214"/>
+    </row>
+    <row r="45" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="22">
         <v>43</v>
       </c>
@@ -3971,12 +3971,12 @@
       <c r="P45" s="46">
         <v>42077</v>
       </c>
-      <c r="Q45" s="217">
+      <c r="Q45" s="214">
         <v>6</v>
       </c>
-      <c r="R45" s="217"/>
-    </row>
-    <row r="46" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R45" s="214"/>
+    </row>
+    <row r="46" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="10">
         <v>44</v>
       </c>
@@ -4005,12 +4005,12 @@
       <c r="P46" s="46">
         <v>42084</v>
       </c>
-      <c r="Q46" s="217">
+      <c r="Q46" s="214">
         <v>7</v>
       </c>
-      <c r="R46" s="217"/>
-    </row>
-    <row r="47" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R46" s="214"/>
+    </row>
+    <row r="47" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="11">
         <v>45</v>
       </c>
@@ -4055,12 +4055,12 @@
       <c r="P47" s="46">
         <v>42091</v>
       </c>
-      <c r="Q47" s="217">
+      <c r="Q47" s="214">
         <v>8</v>
       </c>
-      <c r="R47" s="217"/>
-    </row>
-    <row r="48" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R47" s="214"/>
+    </row>
+    <row r="48" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="11">
         <v>46</v>
       </c>
@@ -4095,12 +4095,12 @@
       <c r="P48" s="46">
         <v>42098</v>
       </c>
-      <c r="Q48" s="217">
+      <c r="Q48" s="214">
         <v>9</v>
       </c>
-      <c r="R48" s="217"/>
-    </row>
-    <row r="49" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R48" s="214"/>
+    </row>
+    <row r="49" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="22">
         <v>47</v>
       </c>
@@ -4145,12 +4145,12 @@
       <c r="P49" s="46">
         <v>42105</v>
       </c>
-      <c r="Q49" s="217">
+      <c r="Q49" s="214">
         <v>10</v>
       </c>
-      <c r="R49" s="217"/>
-    </row>
-    <row r="50" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R49" s="214"/>
+    </row>
+    <row r="50" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="22">
         <v>48</v>
       </c>
@@ -4195,12 +4195,12 @@
       <c r="P50" s="46">
         <v>42112</v>
       </c>
-      <c r="Q50" s="217">
+      <c r="Q50" s="214">
         <v>11</v>
       </c>
-      <c r="R50" s="217"/>
-    </row>
-    <row r="51" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R50" s="214"/>
+    </row>
+    <row r="51" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="11">
         <v>49</v>
       </c>
@@ -4231,12 +4231,12 @@
       <c r="P51" s="46">
         <v>42119</v>
       </c>
-      <c r="Q51" s="217">
+      <c r="Q51" s="214">
         <v>12</v>
       </c>
-      <c r="R51" s="217"/>
-    </row>
-    <row r="52" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R51" s="214"/>
+    </row>
+    <row r="52" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="22">
         <v>50</v>
       </c>
@@ -4281,12 +4281,12 @@
       <c r="P52" s="46">
         <v>42126</v>
       </c>
-      <c r="Q52" s="217">
+      <c r="Q52" s="214">
         <v>13</v>
       </c>
-      <c r="R52" s="217"/>
-    </row>
-    <row r="53" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R52" s="214"/>
+    </row>
+    <row r="53" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="22">
         <v>51</v>
       </c>
@@ -4331,12 +4331,12 @@
       <c r="P53" s="46">
         <v>42133</v>
       </c>
-      <c r="Q53" s="217">
+      <c r="Q53" s="214">
         <v>14</v>
       </c>
-      <c r="R53" s="217"/>
-    </row>
-    <row r="54" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R53" s="214"/>
+    </row>
+    <row r="54" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="22">
         <v>52</v>
       </c>
@@ -4381,12 +4381,12 @@
       <c r="P54" s="46">
         <v>42140</v>
       </c>
-      <c r="Q54" s="217">
+      <c r="Q54" s="214">
         <v>15</v>
       </c>
-      <c r="R54" s="217"/>
-    </row>
-    <row r="55" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R54" s="214"/>
+    </row>
+    <row r="55" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="22">
         <v>53</v>
       </c>
@@ -4431,12 +4431,12 @@
       <c r="P55" s="46">
         <v>42147</v>
       </c>
-      <c r="Q55" s="217">
+      <c r="Q55" s="214">
         <v>16</v>
       </c>
-      <c r="R55" s="217"/>
-    </row>
-    <row r="56" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R55" s="214"/>
+    </row>
+    <row r="56" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="10">
         <v>54</v>
       </c>
@@ -4465,12 +4465,12 @@
       <c r="P56" s="46">
         <v>42154</v>
       </c>
-      <c r="Q56" s="217">
+      <c r="Q56" s="214">
         <v>17</v>
       </c>
-      <c r="R56" s="217"/>
-    </row>
-    <row r="57" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R56" s="214"/>
+    </row>
+    <row r="57" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="11">
         <v>55</v>
       </c>
@@ -4510,7 +4510,7 @@
         <v>49401.041666666672</v>
       </c>
     </row>
-    <row r="58" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="11">
         <v>56</v>
       </c>
@@ -4556,7 +4556,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="59" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="10">
         <v>57</v>
       </c>
@@ -4602,7 +4602,7 @@
         <v>1693750</v>
       </c>
     </row>
-    <row r="60" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="10">
         <v>58</v>
       </c>
@@ -4633,7 +4633,7 @@
         <v>56458.333333333336</v>
       </c>
     </row>
-    <row r="61" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="11">
         <v>59</v>
       </c>
@@ -4680,7 +4680,7 @@
         <v>7057.291666666667</v>
       </c>
     </row>
-    <row r="62" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="11">
         <v>60</v>
       </c>
@@ -4720,7 +4720,7 @@
         <v>42343.75</v>
       </c>
     </row>
-    <row r="63" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="11">
         <v>61</v>
       </c>
@@ -4760,7 +4760,7 @@
         <v>70572.916666666672</v>
       </c>
     </row>
-    <row r="64" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="11">
         <v>62</v>
       </c>
@@ -4800,7 +4800,7 @@
         <v>5292.96875</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="11">
         <v>63</v>
       </c>
@@ -4840,7 +4840,7 @@
         <v>63515.625</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="189">
         <v>64</v>
       </c>
@@ -4880,7 +4880,7 @@
         <v>190546.875</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="192">
         <v>65</v>
       </c>
@@ -4920,7 +4920,7 @@
         <v>3528.6458333333335</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="K68" s="47"/>
       <c r="L68" s="48">
         <f>SUM(L61:L67)+L59+L58+L57+L55+L54+L53+L52+L50+L49+L48+L47+L45+L44+L43+L42+L38+L37+L36+L33+L32+L31+L30+L29+L25+L24+L22+L21+L20+L19+L18+SUM(L3:L15)</f>
@@ -4929,26 +4929,26 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="Q40:R40"/>
+    <mergeCell ref="O39:P39"/>
+    <mergeCell ref="Q39:R39"/>
+    <mergeCell ref="Q41:R41"/>
+    <mergeCell ref="Q42:R42"/>
+    <mergeCell ref="Q43:R43"/>
+    <mergeCell ref="Q44:R44"/>
+    <mergeCell ref="Q45:R45"/>
+    <mergeCell ref="Q46:R46"/>
+    <mergeCell ref="Q47:R47"/>
+    <mergeCell ref="Q48:R48"/>
+    <mergeCell ref="Q49:R49"/>
+    <mergeCell ref="Q50:R50"/>
+    <mergeCell ref="Q51:R51"/>
     <mergeCell ref="Q52:R52"/>
     <mergeCell ref="Q53:R53"/>
     <mergeCell ref="Q54:R54"/>
     <mergeCell ref="Q55:R55"/>
     <mergeCell ref="Q56:R56"/>
-    <mergeCell ref="Q47:R47"/>
-    <mergeCell ref="Q48:R48"/>
-    <mergeCell ref="Q49:R49"/>
-    <mergeCell ref="Q50:R50"/>
-    <mergeCell ref="Q51:R51"/>
-    <mergeCell ref="Q42:R42"/>
-    <mergeCell ref="Q43:R43"/>
-    <mergeCell ref="Q44:R44"/>
-    <mergeCell ref="Q45:R45"/>
-    <mergeCell ref="Q46:R46"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="Q40:R40"/>
-    <mergeCell ref="O39:P39"/>
-    <mergeCell ref="Q39:R39"/>
-    <mergeCell ref="Q41:R41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -4959,34 +4959,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R71"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="17.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="19.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" style="50" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="64.28515625" style="50" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" style="50" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" style="50" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" style="50" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="50" customWidth="1"/>
+    <col min="1" max="1" width="4.5546875" style="50" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.33203125" style="50" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" style="50" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.109375" style="50" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" style="50" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" style="50" customWidth="1"/>
     <col min="7" max="7" width="16" style="50" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" style="50" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" style="50" customWidth="1"/>
-    <col min="10" max="10" width="32.28515625" style="50" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="47.42578125" style="50" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.42578125" style="50" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" style="50" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.42578125" style="50" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="62.42578125" style="50" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" style="50" customWidth="1"/>
-    <col min="17" max="17" width="9.7109375" style="50" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.88671875" style="50" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" style="50" customWidth="1"/>
+    <col min="10" max="10" width="32.33203125" style="50" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="47.44140625" style="50" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.44140625" style="50" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" style="50" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.44140625" style="50" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="62.44140625" style="50" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" style="50" customWidth="1"/>
+    <col min="17" max="17" width="9.6640625" style="50" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="31" style="50" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="11.5703125" style="50"/>
+    <col min="19" max="16384" width="11.5546875" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="218" t="s">
         <v>113</v>
       </c>
@@ -5002,7 +5002,7 @@
       <c r="K1" s="219"/>
       <c r="L1" s="220"/>
     </row>
-    <row r="2" spans="1:18" ht="69.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="77.400000000000006" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="79" t="s">
         <v>0</v>
       </c>
@@ -5046,7 +5046,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="51">
         <v>1</v>
       </c>
@@ -5094,7 +5094,7 @@
       <c r="Q3" s="54"/>
       <c r="R3" s="55"/>
     </row>
-    <row r="4" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="61">
         <v>2</v>
       </c>
@@ -5142,7 +5142,7 @@
       <c r="Q4" s="59"/>
       <c r="R4" s="60"/>
     </row>
-    <row r="5" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="87">
         <v>3</v>
       </c>
@@ -5223,7 +5223,7 @@
       <c r="Q6" s="64"/>
       <c r="R6" s="65"/>
     </row>
-    <row r="7" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="87">
         <v>5</v>
       </c>
@@ -5265,7 +5265,7 @@
       <c r="Q7" s="66"/>
       <c r="R7" s="67"/>
     </row>
-    <row r="8" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="87">
         <v>6</v>
       </c>
@@ -5312,7 +5312,7 @@
         <v>42084</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="87">
         <v>7</v>
       </c>
@@ -5332,8 +5332,8 @@
         <f>D9*(C9*30 +E9*30)/60</f>
         <v>18</v>
       </c>
-      <c r="G9" s="51" t="s">
-        <v>152</v>
+      <c r="G9" s="51">
+        <v>20</v>
       </c>
       <c r="H9" s="69">
         <v>42091</v>
@@ -5389,7 +5389,7 @@
         <v>42098</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="87">
         <v>9</v>
       </c>
@@ -5426,7 +5426,7 @@
         <v>42105</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="87">
         <v>10</v>
       </c>
@@ -5439,8 +5439,8 @@
       <c r="F12" s="61">
         <v>2</v>
       </c>
-      <c r="G12" s="51" t="s">
-        <v>152</v>
+      <c r="G12" s="51">
+        <v>5</v>
       </c>
       <c r="H12" s="69">
         <v>42091</v>
@@ -5465,7 +5465,7 @@
         <v>42112</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="38.4" x14ac:dyDescent="0.3">
       <c r="A13" s="87">
         <v>11</v>
       </c>
@@ -5485,8 +5485,8 @@
         <f>40*C13</f>
         <v>120</v>
       </c>
-      <c r="G13" s="51" t="s">
-        <v>152</v>
+      <c r="G13" s="51">
+        <v>100</v>
       </c>
       <c r="H13" s="69">
         <v>42091</v>
@@ -5511,7 +5511,7 @@
         <v>42119</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="38.4" x14ac:dyDescent="0.3">
       <c r="A14" s="87">
         <v>12</v>
       </c>
@@ -5524,8 +5524,8 @@
       <c r="F14" s="61">
         <v>3</v>
       </c>
-      <c r="G14" s="51" t="s">
-        <v>152</v>
+      <c r="G14" s="51">
+        <v>3</v>
       </c>
       <c r="H14" s="69">
         <v>42091</v>
@@ -5550,7 +5550,7 @@
         <v>42126</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="117">
         <v>13</v>
       </c>
@@ -5563,8 +5563,8 @@
       <c r="F15" s="117">
         <v>3</v>
       </c>
-      <c r="G15" s="117" t="s">
-        <v>152</v>
+      <c r="G15" s="117">
+        <v>3</v>
       </c>
       <c r="H15" s="128">
         <v>42091</v>
@@ -5589,7 +5589,7 @@
         <v>42133</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="117">
         <v>14</v>
       </c>
@@ -5602,8 +5602,8 @@
       <c r="F16" s="117">
         <v>2</v>
       </c>
-      <c r="G16" s="117" t="s">
-        <v>152</v>
+      <c r="G16" s="117">
+        <v>2</v>
       </c>
       <c r="H16" s="128">
         <v>42111</v>
@@ -5628,14 +5628,20 @@
         <v>42140</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A17" s="97"/>
       <c r="B17" s="91"/>
       <c r="C17" s="91"/>
       <c r="D17" s="91"/>
       <c r="E17" s="91"/>
-      <c r="F17" s="91"/>
-      <c r="G17" s="92"/>
+      <c r="F17" s="91">
+        <f>SUM(F3:F16)</f>
+        <v>169.5</v>
+      </c>
+      <c r="G17" s="92">
+        <f>SUM(G3:G16)</f>
+        <v>153</v>
+      </c>
       <c r="H17" s="93"/>
       <c r="I17" s="93"/>
       <c r="J17" s="92"/>
@@ -5653,7 +5659,7 @@
         <v>42147</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A18" s="97"/>
       <c r="B18" s="91"/>
       <c r="C18" s="92"/>
@@ -5673,7 +5679,7 @@
         <v>42154</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A19" s="97"/>
       <c r="B19" s="91"/>
       <c r="C19" s="92"/>
@@ -5701,7 +5707,7 @@
       <c r="K20" s="92"/>
       <c r="L20" s="94"/>
     </row>
-    <row r="21" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="97"/>
       <c r="B21" s="96"/>
       <c r="C21" s="92"/>
@@ -5721,7 +5727,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A22" s="97"/>
       <c r="B22" s="209"/>
       <c r="C22" s="92"/>
@@ -5742,7 +5748,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="38.4" x14ac:dyDescent="0.3">
       <c r="A23" s="92"/>
       <c r="B23" s="96"/>
       <c r="C23" s="92"/>
@@ -5763,7 +5769,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="92"/>
       <c r="B24" s="96"/>
       <c r="C24" s="92"/>
@@ -5784,7 +5790,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="97"/>
       <c r="B25" s="211"/>
       <c r="C25" s="91"/>
@@ -5805,7 +5811,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A26" s="97"/>
       <c r="B26" s="213"/>
       <c r="C26" s="92"/>
@@ -5820,7 +5826,7 @@
       <c r="L26" s="212"/>
       <c r="M26" s="91"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A27" s="97"/>
       <c r="B27" s="213"/>
       <c r="C27" s="92"/>
@@ -5835,7 +5841,7 @@
       <c r="L27" s="212"/>
       <c r="M27" s="91"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A28" s="92"/>
       <c r="B28" s="96"/>
       <c r="C28" s="92"/>
@@ -5850,7 +5856,7 @@
       <c r="L28" s="94"/>
       <c r="M28" s="91"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A29" s="92"/>
       <c r="B29" s="96"/>
       <c r="C29" s="92"/>
@@ -5865,7 +5871,7 @@
       <c r="L29" s="94"/>
       <c r="M29" s="91"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A30" s="92"/>
       <c r="B30" s="96"/>
       <c r="C30" s="92"/>
@@ -5880,7 +5886,7 @@
       <c r="L30" s="94"/>
       <c r="M30" s="91"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A31" s="92"/>
       <c r="B31" s="96"/>
       <c r="C31" s="92"/>
@@ -5894,7 +5900,7 @@
       <c r="K31" s="92"/>
       <c r="L31" s="94"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A32" s="92"/>
       <c r="B32" s="96"/>
       <c r="C32" s="92"/>
@@ -5908,7 +5914,7 @@
       <c r="K32" s="92"/>
       <c r="L32" s="94"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="92"/>
       <c r="B33" s="96"/>
       <c r="C33" s="92"/>
@@ -5922,7 +5928,7 @@
       <c r="K33" s="92"/>
       <c r="L33" s="94"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="92"/>
       <c r="B34" s="96"/>
       <c r="C34" s="92"/>
@@ -5936,7 +5942,7 @@
       <c r="K34" s="92"/>
       <c r="L34" s="94"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="92"/>
       <c r="B35" s="95"/>
       <c r="C35" s="92"/>
@@ -5950,7 +5956,7 @@
       <c r="K35" s="92"/>
       <c r="L35" s="94"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="92"/>
       <c r="B36" s="96"/>
       <c r="C36" s="92"/>
@@ -5964,7 +5970,7 @@
       <c r="K36" s="92"/>
       <c r="L36" s="94"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="92"/>
       <c r="B37" s="96"/>
       <c r="C37" s="92"/>
@@ -5978,7 +5984,7 @@
       <c r="K37" s="92"/>
       <c r="L37" s="94"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="92"/>
       <c r="B38" s="96"/>
       <c r="C38" s="92"/>
@@ -5992,7 +5998,7 @@
       <c r="K38" s="92"/>
       <c r="L38" s="94"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="92"/>
       <c r="B39" s="96"/>
       <c r="C39" s="92"/>
@@ -6006,7 +6012,7 @@
       <c r="K39" s="92"/>
       <c r="L39" s="94"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="92"/>
       <c r="B40" s="96"/>
       <c r="C40" s="92"/>
@@ -6020,7 +6026,7 @@
       <c r="K40" s="92"/>
       <c r="L40" s="94"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="92"/>
       <c r="B41" s="96"/>
       <c r="C41" s="92"/>
@@ -6034,7 +6040,7 @@
       <c r="K41" s="92"/>
       <c r="L41" s="94"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="92"/>
       <c r="B42" s="96"/>
       <c r="C42" s="92"/>
@@ -6048,7 +6054,7 @@
       <c r="K42" s="92"/>
       <c r="L42" s="94"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="92"/>
       <c r="B43" s="96"/>
       <c r="C43" s="92"/>
@@ -6062,7 +6068,7 @@
       <c r="K43" s="92"/>
       <c r="L43" s="94"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="92"/>
       <c r="B44" s="96"/>
       <c r="C44" s="92"/>
@@ -6076,7 +6082,7 @@
       <c r="K44" s="92"/>
       <c r="L44" s="94"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="92"/>
       <c r="B45" s="96"/>
       <c r="C45" s="92"/>
@@ -6090,7 +6096,7 @@
       <c r="K45" s="92"/>
       <c r="L45" s="94"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="92"/>
       <c r="B46" s="96"/>
       <c r="C46" s="92"/>
@@ -6104,7 +6110,7 @@
       <c r="K46" s="92"/>
       <c r="L46" s="94"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="92"/>
       <c r="B47" s="96"/>
       <c r="C47" s="92"/>
@@ -6118,7 +6124,7 @@
       <c r="K47" s="92"/>
       <c r="L47" s="94"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="92"/>
       <c r="B48" s="95"/>
       <c r="C48" s="92"/>
@@ -6132,7 +6138,7 @@
       <c r="K48" s="92"/>
       <c r="L48" s="94"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="92"/>
       <c r="B49" s="96"/>
       <c r="C49" s="92"/>
@@ -6146,7 +6152,7 @@
       <c r="K49" s="92"/>
       <c r="L49" s="94"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="92"/>
       <c r="B50" s="96"/>
       <c r="C50" s="92"/>
@@ -6160,7 +6166,7 @@
       <c r="K50" s="92"/>
       <c r="L50" s="94"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="92"/>
       <c r="B51" s="96"/>
       <c r="C51" s="92"/>
@@ -6174,7 +6180,7 @@
       <c r="K51" s="92"/>
       <c r="L51" s="94"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="92"/>
       <c r="B52" s="96"/>
       <c r="C52" s="92"/>
@@ -6188,7 +6194,7 @@
       <c r="K52" s="92"/>
       <c r="L52" s="94"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="92"/>
       <c r="B53" s="96"/>
       <c r="C53" s="92"/>
@@ -6202,7 +6208,7 @@
       <c r="K53" s="92"/>
       <c r="L53" s="94"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="92"/>
       <c r="B54" s="96"/>
       <c r="C54" s="92"/>
@@ -6216,7 +6222,7 @@
       <c r="K54" s="92"/>
       <c r="L54" s="94"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="92"/>
       <c r="B55" s="96"/>
       <c r="C55" s="92"/>
@@ -6230,7 +6236,7 @@
       <c r="K55" s="92"/>
       <c r="L55" s="94"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="92"/>
       <c r="B56" s="96"/>
       <c r="C56" s="92"/>
@@ -6244,7 +6250,7 @@
       <c r="K56" s="92"/>
       <c r="L56" s="94"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="92"/>
       <c r="B57" s="96"/>
       <c r="C57" s="92"/>
@@ -6258,7 +6264,7 @@
       <c r="K57" s="92"/>
       <c r="L57" s="94"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="92"/>
       <c r="B58" s="96"/>
       <c r="C58" s="92"/>
@@ -6272,7 +6278,7 @@
       <c r="K58" s="92"/>
       <c r="L58" s="94"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="92"/>
       <c r="B59" s="96"/>
       <c r="C59" s="92"/>
@@ -6286,7 +6292,7 @@
       <c r="K59" s="92"/>
       <c r="L59" s="94"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="92"/>
       <c r="B60" s="96"/>
       <c r="C60" s="92"/>
@@ -6300,7 +6306,7 @@
       <c r="K60" s="92"/>
       <c r="L60" s="94"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="92"/>
       <c r="B61" s="92"/>
       <c r="C61" s="92"/>
@@ -6314,7 +6320,7 @@
       <c r="K61" s="92"/>
       <c r="L61" s="94"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="92"/>
       <c r="B62" s="92"/>
       <c r="C62" s="92"/>
@@ -6328,7 +6334,7 @@
       <c r="K62" s="92"/>
       <c r="L62" s="94"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="92"/>
       <c r="B63" s="92"/>
       <c r="C63" s="92"/>
@@ -6342,7 +6348,7 @@
       <c r="K63" s="92"/>
       <c r="L63" s="94"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="92"/>
       <c r="B64" s="92"/>
       <c r="C64" s="92"/>
@@ -6356,7 +6362,7 @@
       <c r="K64" s="92"/>
       <c r="L64" s="94"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="92"/>
       <c r="B65" s="92"/>
       <c r="C65" s="92"/>
@@ -6370,7 +6376,7 @@
       <c r="K65" s="92"/>
       <c r="L65" s="94"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="92"/>
       <c r="B66" s="92"/>
       <c r="C66" s="92"/>
@@ -6384,7 +6390,7 @@
       <c r="K66" s="92"/>
       <c r="L66" s="94"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="92"/>
       <c r="B67" s="92"/>
       <c r="C67" s="92"/>
@@ -6398,19 +6404,19 @@
       <c r="K67" s="92"/>
       <c r="L67" s="94"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="92"/>
       <c r="B68" s="91"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="91"/>
       <c r="B69" s="91"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="91"/>
       <c r="B70" s="91"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="91"/>
       <c r="B71" s="91"/>
     </row>
@@ -6427,32 +6433,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R74"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="17.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="19.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" style="50" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.140625" style="50" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="50" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="50" customWidth="1"/>
-    <col min="5" max="6" width="16.5703125" style="50" customWidth="1"/>
+    <col min="1" max="1" width="4.5546875" style="50" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.109375" style="50" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" style="50" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="50" customWidth="1"/>
+    <col min="5" max="6" width="16.5546875" style="50" customWidth="1"/>
     <col min="7" max="7" width="16" style="50" customWidth="1"/>
-    <col min="8" max="9" width="18.42578125" style="50" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="18.44140625" style="50" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="29" style="50" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="57.28515625" style="50" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.42578125" style="50" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" style="50" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.42578125" style="50" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="62.42578125" style="50" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" style="50" customWidth="1"/>
-    <col min="17" max="17" width="9.7109375" style="50" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="57.33203125" style="50" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.44140625" style="50" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" style="50" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.44140625" style="50" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="62.44140625" style="50" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" style="50" customWidth="1"/>
+    <col min="17" max="17" width="9.6640625" style="50" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="31" style="50" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="11.5703125" style="50"/>
+    <col min="19" max="16384" width="11.5546875" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="221" t="s">
         <v>113</v>
       </c>
@@ -6468,7 +6474,7 @@
       <c r="K1" s="221"/>
       <c r="L1" s="221"/>
     </row>
-    <row r="2" spans="1:18" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="116" t="s">
         <v>0</v>
       </c>
@@ -6512,7 +6518,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="51">
         <v>1</v>
       </c>
@@ -6525,8 +6531,8 @@
       <c r="F3" s="61">
         <v>0.5</v>
       </c>
-      <c r="G3" s="61" t="s">
-        <v>152</v>
+      <c r="G3" s="61">
+        <v>1</v>
       </c>
       <c r="H3" s="69">
         <v>42105</v>
@@ -6577,7 +6583,7 @@
       <c r="Q4" s="59"/>
       <c r="R4" s="60"/>
     </row>
-    <row r="5" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="87">
         <v>3</v>
       </c>
@@ -6597,8 +6603,8 @@
         <f>D5*(C5*30 +E5*30)/60</f>
         <v>6</v>
       </c>
-      <c r="G5" s="61" t="s">
-        <v>152</v>
+      <c r="G5" s="61">
+        <v>15</v>
       </c>
       <c r="H5" s="69">
         <v>42109</v>
@@ -6626,7 +6632,7 @@
       <c r="Q5" s="63"/>
       <c r="R5" s="60"/>
     </row>
-    <row r="6" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="87">
         <v>4</v>
       </c>
@@ -6646,8 +6652,8 @@
         <f t="shared" ref="F6" si="1">D6*(C6*30 +E6*30)/60</f>
         <v>23</v>
       </c>
-      <c r="G6" s="61" t="s">
-        <v>152</v>
+      <c r="G6" s="61">
+        <v>25</v>
       </c>
       <c r="H6" s="69">
         <v>42109</v>
@@ -6675,7 +6681,7 @@
       <c r="Q6" s="64"/>
       <c r="R6" s="65"/>
     </row>
-    <row r="7" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="51">
         <v>5</v>
       </c>
@@ -6695,8 +6701,8 @@
         <f>D7*(C7*30 +E7*30)/60</f>
         <v>0.5</v>
       </c>
-      <c r="G7" s="51" t="s">
-        <v>152</v>
+      <c r="G7" s="51">
+        <v>2</v>
       </c>
       <c r="H7" s="69">
         <v>42091</v>
@@ -6719,7 +6725,7 @@
       <c r="Q7" s="201"/>
       <c r="R7" s="202"/>
     </row>
-    <row r="8" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="61">
         <v>6</v>
       </c>
@@ -6739,8 +6745,8 @@
         <f>D8*(C8*30 +E8*30)/60</f>
         <v>6</v>
       </c>
-      <c r="G8" s="51" t="s">
-        <v>152</v>
+      <c r="G8" s="51">
+        <v>4</v>
       </c>
       <c r="H8" s="69">
         <v>42091</v>
@@ -6763,7 +6769,7 @@
       <c r="Q8" s="201"/>
       <c r="R8" s="202"/>
     </row>
-    <row r="9" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="87">
         <v>7</v>
       </c>
@@ -6783,8 +6789,8 @@
         <f>D9*(C9*30 +E9*30)/60</f>
         <v>18</v>
       </c>
-      <c r="G9" s="51" t="s">
-        <v>152</v>
+      <c r="G9" s="51">
+        <v>16</v>
       </c>
       <c r="H9" s="69">
         <v>42091</v>
@@ -6832,7 +6838,7 @@
         <v>42084</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="51">
         <v>9</v>
       </c>
@@ -6845,8 +6851,8 @@
       <c r="F11" s="61">
         <v>2</v>
       </c>
-      <c r="G11" s="61" t="s">
-        <v>152</v>
+      <c r="G11" s="61">
+        <v>5</v>
       </c>
       <c r="H11" s="69">
         <v>42107</v>
@@ -6869,7 +6875,7 @@
         <v>42091</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="61">
         <v>10</v>
       </c>
@@ -6882,8 +6888,8 @@
       <c r="F12" s="61">
         <v>2</v>
       </c>
-      <c r="G12" s="61" t="s">
-        <v>152</v>
+      <c r="G12" s="61">
+        <v>2</v>
       </c>
       <c r="H12" s="69">
         <v>42107</v>
@@ -6908,7 +6914,7 @@
         <v>42098</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="87">
         <v>11</v>
       </c>
@@ -6921,8 +6927,8 @@
       <c r="F13" s="61">
         <v>2</v>
       </c>
-      <c r="G13" s="61" t="s">
-        <v>152</v>
+      <c r="G13" s="61">
+        <v>2</v>
       </c>
       <c r="H13" s="69">
         <v>42107</v>
@@ -6947,7 +6953,7 @@
         <v>42105</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="87">
         <v>12</v>
       </c>
@@ -6967,8 +6973,8 @@
         <f>40*C14</f>
         <v>120</v>
       </c>
-      <c r="G14" s="61" t="s">
-        <v>152</v>
+      <c r="G14" s="61">
+        <v>120</v>
       </c>
       <c r="H14" s="69">
         <v>42107</v>
@@ -6993,7 +6999,7 @@
         <v>42112</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="51">
         <v>13</v>
       </c>
@@ -7006,8 +7012,8 @@
       <c r="F15" s="61">
         <v>3</v>
       </c>
-      <c r="G15" s="61" t="s">
-        <v>152</v>
+      <c r="G15" s="61">
+        <v>2</v>
       </c>
       <c r="H15" s="69">
         <v>42107</v>
@@ -7032,7 +7038,7 @@
         <v>42119</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="61">
         <v>14</v>
       </c>
@@ -7045,8 +7051,8 @@
       <c r="F16" s="61">
         <v>3</v>
       </c>
-      <c r="G16" s="61" t="s">
-        <v>152</v>
+      <c r="G16" s="61">
+        <v>3</v>
       </c>
       <c r="H16" s="69">
         <v>42107</v>
@@ -7071,7 +7077,7 @@
         <v>42126</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="117">
         <v>15</v>
       </c>
@@ -7090,8 +7096,8 @@
       <c r="F17" s="117">
         <v>3</v>
       </c>
-      <c r="G17" s="117" t="s">
-        <v>152</v>
+      <c r="G17" s="117">
+        <v>4</v>
       </c>
       <c r="H17" s="128">
         <v>42113</v>
@@ -7116,7 +7122,7 @@
         <v>42133</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="117">
         <v>16</v>
       </c>
@@ -7129,8 +7135,8 @@
       <c r="F18" s="117">
         <v>2</v>
       </c>
-      <c r="G18" s="117" t="s">
-        <v>152</v>
+      <c r="G18" s="117">
+        <v>2</v>
       </c>
       <c r="H18" s="128">
         <v>42115</v>
@@ -7155,8 +7161,16 @@
         <v>42140</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A19" s="97"/>
+      <c r="F19" s="50">
+        <f>SUM(F3:F18)</f>
+        <v>191</v>
+      </c>
+      <c r="G19" s="50">
+        <f>SUM(G3:G18)</f>
+        <v>203</v>
+      </c>
       <c r="K19" s="129" t="s">
         <v>163</v>
       </c>
@@ -7172,7 +7186,7 @@
         <v>42147</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A20" s="97"/>
       <c r="B20" s="125"/>
       <c r="C20" s="97"/>
@@ -7193,7 +7207,7 @@
         <v>42154</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A21" s="97"/>
       <c r="B21" s="125"/>
       <c r="C21" s="97"/>
@@ -7227,7 +7241,7 @@
       <c r="N22" s="101"/>
       <c r="O22" s="101"/>
     </row>
-    <row r="23" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="97"/>
       <c r="B23" s="125"/>
       <c r="C23" s="97"/>
@@ -7248,7 +7262,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A24" s="97"/>
       <c r="B24" s="125"/>
       <c r="C24" s="97"/>
@@ -7269,7 +7283,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="38.4" x14ac:dyDescent="0.3">
       <c r="A25" s="97"/>
       <c r="B25" s="125"/>
       <c r="C25" s="97"/>
@@ -7290,7 +7304,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="97"/>
       <c r="B26" s="125"/>
       <c r="C26" s="97"/>
@@ -7311,7 +7325,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="97"/>
       <c r="B27" s="125"/>
       <c r="C27" s="97"/>
@@ -7332,7 +7346,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A28" s="97"/>
       <c r="B28" s="125"/>
       <c r="C28" s="97"/>
@@ -7349,7 +7363,7 @@
       <c r="N28" s="101"/>
       <c r="O28" s="101"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A29" s="97"/>
       <c r="B29" s="125"/>
       <c r="C29" s="97"/>
@@ -7366,7 +7380,7 @@
       <c r="N29" s="101"/>
       <c r="O29" s="101"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A30" s="97"/>
       <c r="B30" s="125"/>
       <c r="C30" s="97"/>
@@ -7383,7 +7397,7 @@
       <c r="N30" s="101"/>
       <c r="O30" s="101"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A31" s="97"/>
       <c r="B31" s="125"/>
       <c r="C31" s="97"/>
@@ -7400,7 +7414,7 @@
       <c r="N31" s="101"/>
       <c r="O31" s="101"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="97"/>
       <c r="B32" s="125"/>
       <c r="C32" s="97"/>
@@ -7417,7 +7431,7 @@
       <c r="N32" s="101"/>
       <c r="O32" s="101"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="97"/>
       <c r="B33" s="125"/>
       <c r="C33" s="97"/>
@@ -7434,7 +7448,7 @@
       <c r="N33" s="101"/>
       <c r="O33" s="101"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="97"/>
       <c r="B34" s="125"/>
       <c r="C34" s="97"/>
@@ -7451,7 +7465,7 @@
       <c r="N34" s="101"/>
       <c r="O34" s="101"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="97"/>
       <c r="B35" s="125"/>
       <c r="C35" s="97"/>
@@ -7468,7 +7482,7 @@
       <c r="N35" s="101"/>
       <c r="O35" s="101"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="97"/>
       <c r="B36" s="125"/>
       <c r="C36" s="97"/>
@@ -7485,7 +7499,7 @@
       <c r="N36" s="101"/>
       <c r="O36" s="101"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="97"/>
       <c r="B37" s="125"/>
       <c r="C37" s="97"/>
@@ -7502,7 +7516,7 @@
       <c r="N37" s="101"/>
       <c r="O37" s="101"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="97"/>
       <c r="B38" s="125"/>
       <c r="C38" s="97"/>
@@ -7519,7 +7533,7 @@
       <c r="N38" s="101"/>
       <c r="O38" s="101"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="97"/>
       <c r="B39" s="125"/>
       <c r="C39" s="97"/>
@@ -7536,7 +7550,7 @@
       <c r="N39" s="101"/>
       <c r="O39" s="101"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" s="97"/>
       <c r="B40" s="125"/>
       <c r="C40" s="97"/>
@@ -7553,7 +7567,7 @@
       <c r="N40" s="101"/>
       <c r="O40" s="101"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" s="97"/>
       <c r="B41" s="125"/>
       <c r="C41" s="97"/>
@@ -7570,7 +7584,7 @@
       <c r="N41" s="101"/>
       <c r="O41" s="101"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" s="97"/>
       <c r="B42" s="125"/>
       <c r="C42" s="97"/>
@@ -7587,7 +7601,7 @@
       <c r="N42" s="101"/>
       <c r="O42" s="101"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="97"/>
       <c r="B43" s="125"/>
       <c r="C43" s="97"/>
@@ -7604,7 +7618,7 @@
       <c r="N43" s="101"/>
       <c r="O43" s="101"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" s="97"/>
       <c r="B44" s="125"/>
       <c r="C44" s="97"/>
@@ -7621,7 +7635,7 @@
       <c r="N44" s="101"/>
       <c r="O44" s="101"/>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" s="97"/>
       <c r="B45" s="125"/>
       <c r="C45" s="97"/>
@@ -7638,7 +7652,7 @@
       <c r="N45" s="101"/>
       <c r="O45" s="101"/>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" s="97"/>
       <c r="B46" s="125"/>
       <c r="C46" s="97"/>
@@ -7655,7 +7669,7 @@
       <c r="N46" s="101"/>
       <c r="O46" s="101"/>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" s="97"/>
       <c r="B47" s="125"/>
       <c r="C47" s="97"/>
@@ -7672,7 +7686,7 @@
       <c r="N47" s="101"/>
       <c r="O47" s="101"/>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" s="97"/>
       <c r="B48" s="125"/>
       <c r="C48" s="97"/>
@@ -7689,7 +7703,7 @@
       <c r="N48" s="101"/>
       <c r="O48" s="101"/>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" s="97"/>
       <c r="B49" s="125"/>
       <c r="C49" s="97"/>
@@ -7706,7 +7720,7 @@
       <c r="N49" s="101"/>
       <c r="O49" s="101"/>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" s="97"/>
       <c r="B50" s="125"/>
       <c r="C50" s="97"/>
@@ -7723,7 +7737,7 @@
       <c r="N50" s="101"/>
       <c r="O50" s="101"/>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" s="97"/>
       <c r="B51" s="125"/>
       <c r="C51" s="97"/>
@@ -7740,7 +7754,7 @@
       <c r="N51" s="101"/>
       <c r="O51" s="101"/>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" s="97"/>
       <c r="B52" s="125"/>
       <c r="C52" s="97"/>
@@ -7757,7 +7771,7 @@
       <c r="N52" s="101"/>
       <c r="O52" s="101"/>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" s="97"/>
       <c r="B53" s="125"/>
       <c r="C53" s="97"/>
@@ -7774,7 +7788,7 @@
       <c r="N53" s="101"/>
       <c r="O53" s="101"/>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" s="97"/>
       <c r="B54" s="125"/>
       <c r="C54" s="97"/>
@@ -7791,7 +7805,7 @@
       <c r="N54" s="101"/>
       <c r="O54" s="101"/>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" s="97"/>
       <c r="B55" s="125"/>
       <c r="C55" s="97"/>
@@ -7808,7 +7822,7 @@
       <c r="N55" s="101"/>
       <c r="O55" s="101"/>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" s="97"/>
       <c r="B56" s="125"/>
       <c r="C56" s="97"/>
@@ -7825,7 +7839,7 @@
       <c r="N56" s="101"/>
       <c r="O56" s="101"/>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" s="97"/>
       <c r="B57" s="125"/>
       <c r="C57" s="97"/>
@@ -7842,7 +7856,7 @@
       <c r="N57" s="101"/>
       <c r="O57" s="101"/>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" s="97"/>
       <c r="B58" s="125"/>
       <c r="C58" s="97"/>
@@ -7859,7 +7873,7 @@
       <c r="N58" s="101"/>
       <c r="O58" s="101"/>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" s="97"/>
       <c r="B59" s="125"/>
       <c r="C59" s="97"/>
@@ -7876,7 +7890,7 @@
       <c r="N59" s="101"/>
       <c r="O59" s="101"/>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" s="97"/>
       <c r="B60" s="125"/>
       <c r="C60" s="97"/>
@@ -7893,7 +7907,7 @@
       <c r="N60" s="101"/>
       <c r="O60" s="101"/>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" s="97"/>
       <c r="B61" s="125"/>
       <c r="C61" s="97"/>
@@ -7910,7 +7924,7 @@
       <c r="N61" s="101"/>
       <c r="O61" s="101"/>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" s="97"/>
       <c r="B62" s="125"/>
       <c r="C62" s="97"/>
@@ -7927,7 +7941,7 @@
       <c r="N62" s="101"/>
       <c r="O62" s="101"/>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" s="97"/>
       <c r="B63" s="97"/>
       <c r="C63" s="97"/>
@@ -7944,7 +7958,7 @@
       <c r="N63" s="101"/>
       <c r="O63" s="101"/>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" s="97"/>
       <c r="B64" s="97"/>
       <c r="C64" s="97"/>
@@ -7961,7 +7975,7 @@
       <c r="N64" s="101"/>
       <c r="O64" s="101"/>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65" s="97"/>
       <c r="B65" s="97"/>
       <c r="C65" s="97"/>
@@ -7978,7 +7992,7 @@
       <c r="N65" s="101"/>
       <c r="O65" s="101"/>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66" s="97"/>
       <c r="B66" s="97"/>
       <c r="C66" s="97"/>
@@ -7995,7 +8009,7 @@
       <c r="N66" s="101"/>
       <c r="O66" s="101"/>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67" s="97"/>
       <c r="B67" s="97"/>
       <c r="C67" s="97"/>
@@ -8012,7 +8026,7 @@
       <c r="N67" s="101"/>
       <c r="O67" s="101"/>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68" s="97"/>
       <c r="B68" s="97"/>
       <c r="C68" s="97"/>
@@ -8029,7 +8043,7 @@
       <c r="N68" s="101"/>
       <c r="O68" s="101"/>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69" s="97"/>
       <c r="B69" s="97"/>
       <c r="C69" s="97"/>
@@ -8046,7 +8060,7 @@
       <c r="N69" s="101"/>
       <c r="O69" s="101"/>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A70" s="97"/>
       <c r="B70" s="97"/>
       <c r="C70" s="97"/>
@@ -8063,7 +8077,7 @@
       <c r="N70" s="101"/>
       <c r="O70" s="101"/>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71" s="97"/>
       <c r="B71" s="97"/>
       <c r="C71" s="97"/>
@@ -8080,7 +8094,7 @@
       <c r="N71" s="101"/>
       <c r="O71" s="101"/>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72" s="97"/>
       <c r="B72" s="97"/>
       <c r="C72" s="97"/>
@@ -8097,7 +8111,7 @@
       <c r="N72" s="101"/>
       <c r="O72" s="101"/>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73" s="97"/>
       <c r="B73" s="97"/>
       <c r="C73" s="97"/>
@@ -8114,7 +8128,7 @@
       <c r="N73" s="101"/>
       <c r="O73" s="101"/>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74" s="97"/>
       <c r="B74" s="97"/>
       <c r="C74" s="101"/>
@@ -8148,30 +8162,30 @@
       <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="17.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="19.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" style="50" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5546875" style="50" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43" style="50" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" style="50" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" style="50" customWidth="1"/>
     <col min="4" max="4" width="19" style="50" customWidth="1"/>
     <col min="5" max="5" width="16" style="50" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" style="50" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" style="50" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" style="50" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" style="50" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" style="50" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" style="50" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" style="50" customWidth="1"/>
+    <col min="9" max="9" width="16.88671875" style="50" customWidth="1"/>
     <col min="10" max="10" width="29" style="50" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="57.28515625" style="50" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.42578125" style="50" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" style="50" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.42578125" style="50" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="62.42578125" style="50" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" style="50" customWidth="1"/>
-    <col min="17" max="17" width="9.7109375" style="50" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="57.33203125" style="50" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.44140625" style="50" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" style="50" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.44140625" style="50" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="62.44140625" style="50" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" style="50" customWidth="1"/>
+    <col min="17" max="17" width="9.6640625" style="50" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="31" style="50" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="11.5703125" style="50"/>
+    <col min="19" max="16384" width="11.5546875" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="218" t="s">
         <v>113</v>
       </c>
@@ -8187,7 +8201,7 @@
       <c r="K1" s="219"/>
       <c r="L1" s="220"/>
     </row>
-    <row r="2" spans="1:18" ht="86.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="86.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="79" t="s">
         <v>0</v>
       </c>
@@ -8231,7 +8245,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="51">
         <v>1</v>
       </c>
@@ -8357,7 +8371,7 @@
       <c r="Q5" s="63"/>
       <c r="R5" s="60"/>
     </row>
-    <row r="6" spans="1:18" s="101" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" s="101" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="87">
         <v>4</v>
       </c>
@@ -8511,7 +8525,7 @@
         <v>42084</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="61">
         <v>8</v>
       </c>
@@ -8635,7 +8649,7 @@
         <v>42105</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="61">
         <v>11</v>
       </c>
@@ -8674,7 +8688,7 @@
         <v>42112</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="61">
         <v>12</v>
       </c>
@@ -8713,7 +8727,7 @@
         <v>42119</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="117">
         <v>13</v>
       </c>
@@ -8789,7 +8803,7 @@
         <v>42140</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A18" s="97"/>
       <c r="B18" s="108"/>
       <c r="C18" s="97"/>
@@ -8810,7 +8824,7 @@
         <v>42147</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A19" s="97"/>
       <c r="B19" s="108"/>
       <c r="C19" s="97"/>
@@ -8831,7 +8845,7 @@
         <v>42154</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A20" s="97"/>
       <c r="B20" s="108"/>
       <c r="C20" s="97"/>
@@ -8861,7 +8875,7 @@
       <c r="L21" s="111"/>
       <c r="M21" s="78"/>
     </row>
-    <row r="22" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="97"/>
       <c r="B22" s="108"/>
       <c r="C22" s="97"/>
@@ -8882,7 +8896,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A23" s="97"/>
       <c r="B23" s="108"/>
       <c r="C23" s="97"/>
@@ -8903,7 +8917,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="38.4" x14ac:dyDescent="0.3">
       <c r="A24" s="97"/>
       <c r="B24" s="108"/>
       <c r="C24" s="97"/>
@@ -8924,7 +8938,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="97"/>
       <c r="B25" s="108"/>
       <c r="C25" s="97"/>
@@ -8945,7 +8959,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="97"/>
       <c r="B26" s="108"/>
       <c r="C26" s="97"/>
@@ -8966,7 +8980,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A27" s="97"/>
       <c r="B27" s="108"/>
       <c r="C27" s="97"/>
@@ -8981,7 +8995,7 @@
       <c r="L27" s="111"/>
       <c r="M27" s="78"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A28" s="97"/>
       <c r="B28" s="108"/>
       <c r="C28" s="97"/>
@@ -8996,7 +9010,7 @@
       <c r="L28" s="111"/>
       <c r="M28" s="78"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A29" s="97"/>
       <c r="B29" s="108"/>
       <c r="C29" s="97"/>
@@ -9011,7 +9025,7 @@
       <c r="L29" s="111"/>
       <c r="M29" s="78"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A30" s="97"/>
       <c r="B30" s="108"/>
       <c r="C30" s="97"/>
@@ -9026,7 +9040,7 @@
       <c r="L30" s="111"/>
       <c r="M30" s="78"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="97"/>
       <c r="B31" s="108"/>
       <c r="C31" s="97"/>
@@ -9041,7 +9055,7 @@
       <c r="L31" s="111"/>
       <c r="M31" s="78"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="97"/>
       <c r="B32" s="108"/>
       <c r="C32" s="97"/>
@@ -9056,7 +9070,7 @@
       <c r="L32" s="111"/>
       <c r="M32" s="78"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="97"/>
       <c r="B33" s="108"/>
       <c r="C33" s="97"/>
@@ -9071,7 +9085,7 @@
       <c r="L33" s="111"/>
       <c r="M33" s="78"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="97"/>
       <c r="B34" s="108"/>
       <c r="C34" s="97"/>
@@ -9086,7 +9100,7 @@
       <c r="L34" s="111"/>
       <c r="M34" s="78"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="97"/>
       <c r="B35" s="108"/>
       <c r="C35" s="97"/>
@@ -9101,7 +9115,7 @@
       <c r="L35" s="111"/>
       <c r="M35" s="78"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="97"/>
       <c r="B36" s="112"/>
       <c r="C36" s="97"/>
@@ -9116,7 +9130,7 @@
       <c r="L36" s="111"/>
       <c r="M36" s="78"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="97"/>
       <c r="B37" s="108"/>
       <c r="C37" s="97"/>
@@ -9131,7 +9145,7 @@
       <c r="L37" s="111"/>
       <c r="M37" s="78"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="97"/>
       <c r="B38" s="108"/>
       <c r="C38" s="97"/>
@@ -9146,7 +9160,7 @@
       <c r="L38" s="111"/>
       <c r="M38" s="78"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="97"/>
       <c r="B39" s="108"/>
       <c r="C39" s="97"/>
@@ -9161,7 +9175,7 @@
       <c r="L39" s="111"/>
       <c r="M39" s="78"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="97"/>
       <c r="B40" s="108"/>
       <c r="C40" s="97"/>
@@ -9176,7 +9190,7 @@
       <c r="L40" s="111"/>
       <c r="M40" s="78"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="97"/>
       <c r="B41" s="108"/>
       <c r="C41" s="97"/>
@@ -9191,7 +9205,7 @@
       <c r="L41" s="111"/>
       <c r="M41" s="78"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="97"/>
       <c r="B42" s="108"/>
       <c r="C42" s="97"/>
@@ -9206,7 +9220,7 @@
       <c r="L42" s="111"/>
       <c r="M42" s="78"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="97"/>
       <c r="B43" s="108"/>
       <c r="C43" s="97"/>
@@ -9221,7 +9235,7 @@
       <c r="L43" s="111"/>
       <c r="M43" s="78"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="97"/>
       <c r="B44" s="108"/>
       <c r="C44" s="97"/>
@@ -9236,7 +9250,7 @@
       <c r="L44" s="111"/>
       <c r="M44" s="78"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="97"/>
       <c r="B45" s="108"/>
       <c r="C45" s="97"/>
@@ -9251,7 +9265,7 @@
       <c r="L45" s="111"/>
       <c r="M45" s="78"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="97"/>
       <c r="B46" s="108"/>
       <c r="C46" s="97"/>
@@ -9266,7 +9280,7 @@
       <c r="L46" s="111"/>
       <c r="M46" s="78"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="97"/>
       <c r="B47" s="108"/>
       <c r="C47" s="97"/>
@@ -9281,7 +9295,7 @@
       <c r="L47" s="111"/>
       <c r="M47" s="78"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="97"/>
       <c r="B48" s="108"/>
       <c r="C48" s="97"/>
@@ -9296,7 +9310,7 @@
       <c r="L48" s="111"/>
       <c r="M48" s="78"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="97"/>
       <c r="B49" s="112"/>
       <c r="C49" s="97"/>
@@ -9311,7 +9325,7 @@
       <c r="L49" s="111"/>
       <c r="M49" s="78"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="97"/>
       <c r="B50" s="108"/>
       <c r="C50" s="97"/>
@@ -9326,7 +9340,7 @@
       <c r="L50" s="111"/>
       <c r="M50" s="78"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="97"/>
       <c r="B51" s="108"/>
       <c r="C51" s="97"/>
@@ -9341,7 +9355,7 @@
       <c r="L51" s="111"/>
       <c r="M51" s="78"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="97"/>
       <c r="B52" s="108"/>
       <c r="C52" s="97"/>
@@ -9356,7 +9370,7 @@
       <c r="L52" s="111"/>
       <c r="M52" s="78"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="97"/>
       <c r="B53" s="108"/>
       <c r="C53" s="97"/>
@@ -9371,7 +9385,7 @@
       <c r="L53" s="111"/>
       <c r="M53" s="78"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="97"/>
       <c r="B54" s="108"/>
       <c r="C54" s="97"/>
@@ -9386,7 +9400,7 @@
       <c r="L54" s="111"/>
       <c r="M54" s="78"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="97"/>
       <c r="B55" s="108"/>
       <c r="C55" s="97"/>
@@ -9401,7 +9415,7 @@
       <c r="L55" s="111"/>
       <c r="M55" s="78"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="97"/>
       <c r="B56" s="108"/>
       <c r="C56" s="97"/>
@@ -9416,7 +9430,7 @@
       <c r="L56" s="111"/>
       <c r="M56" s="78"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="97"/>
       <c r="B57" s="108"/>
       <c r="C57" s="97"/>
@@ -9431,7 +9445,7 @@
       <c r="L57" s="111"/>
       <c r="M57" s="78"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="97"/>
       <c r="B58" s="108"/>
       <c r="C58" s="97"/>
@@ -9446,7 +9460,7 @@
       <c r="L58" s="111"/>
       <c r="M58" s="78"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="97"/>
       <c r="B59" s="108"/>
       <c r="C59" s="97"/>
@@ -9461,7 +9475,7 @@
       <c r="L59" s="111"/>
       <c r="M59" s="78"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="97"/>
       <c r="B60" s="108"/>
       <c r="C60" s="97"/>
@@ -9476,7 +9490,7 @@
       <c r="L60" s="111"/>
       <c r="M60" s="78"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A61" s="97"/>
       <c r="B61" s="108"/>
       <c r="C61" s="97"/>
@@ -9491,7 +9505,7 @@
       <c r="L61" s="111"/>
       <c r="M61" s="78"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" s="97"/>
       <c r="B62" s="97"/>
       <c r="C62" s="97"/>
@@ -9506,7 +9520,7 @@
       <c r="L62" s="111"/>
       <c r="M62" s="78"/>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" s="97"/>
       <c r="B63" s="97"/>
       <c r="C63" s="97"/>
@@ -9521,7 +9535,7 @@
       <c r="L63" s="111"/>
       <c r="M63" s="78"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" s="97"/>
       <c r="B64" s="97"/>
       <c r="C64" s="97"/>
@@ -9536,7 +9550,7 @@
       <c r="L64" s="111"/>
       <c r="M64" s="78"/>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" s="97"/>
       <c r="B65" s="97"/>
       <c r="C65" s="97"/>
@@ -9551,7 +9565,7 @@
       <c r="L65" s="111"/>
       <c r="M65" s="78"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" s="97"/>
       <c r="B66" s="97"/>
       <c r="C66" s="97"/>
@@ -9566,7 +9580,7 @@
       <c r="L66" s="111"/>
       <c r="M66" s="78"/>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" s="97"/>
       <c r="B67" s="97"/>
       <c r="C67" s="97"/>
@@ -9581,7 +9595,7 @@
       <c r="L67" s="111"/>
       <c r="M67" s="78"/>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" s="97"/>
       <c r="B68" s="97"/>
       <c r="C68" s="97"/>
@@ -9596,7 +9610,7 @@
       <c r="L68" s="111"/>
       <c r="M68" s="78"/>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" s="78"/>
       <c r="B69" s="78"/>
       <c r="K69" s="89" t="s">
@@ -9607,11 +9621,11 @@
         <v>1665520.8333333335</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" s="78"/>
       <c r="B70" s="78"/>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" s="78"/>
       <c r="B71" s="78"/>
     </row>
@@ -9628,34 +9642,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" style="133" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" style="133" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" style="133" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="133" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" style="133" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" style="133" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="133" customWidth="1"/>
-    <col min="8" max="8" width="22.85546875" style="133" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" style="133" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.5703125" style="133" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" style="133" customWidth="1"/>
-    <col min="12" max="12" width="26.28515625" style="133" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" style="133" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.42578125" style="133" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="62.42578125" style="133" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" style="133" customWidth="1"/>
-    <col min="17" max="17" width="9.7109375" style="133" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5546875" style="133" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.109375" style="133" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" style="133" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" style="133" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" style="133" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" style="133" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="133" customWidth="1"/>
+    <col min="8" max="8" width="22.88671875" style="133" customWidth="1"/>
+    <col min="9" max="9" width="18.44140625" style="133" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.5546875" style="133" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" style="133" customWidth="1"/>
+    <col min="12" max="12" width="26.33203125" style="133" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" style="133" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.44140625" style="133" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="62.44140625" style="133" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" style="133" customWidth="1"/>
+    <col min="17" max="17" width="9.6640625" style="133" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="31" style="133" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="11.42578125" style="133"/>
+    <col min="19" max="16384" width="11.44140625" style="133"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="222" t="s">
         <v>113</v>
       </c>
@@ -9671,7 +9685,7 @@
       <c r="K1" s="223"/>
       <c r="L1" s="224"/>
     </row>
-    <row r="2" spans="1:18" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="134" t="s">
         <v>0</v>
       </c>
@@ -9715,7 +9729,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="138">
         <v>1</v>
       </c>
@@ -9844,7 +9858,7 @@
       <c r="Q5" s="157"/>
       <c r="R5" s="154"/>
     </row>
-    <row r="6" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="140">
         <v>4</v>
       </c>
@@ -9963,7 +9977,7 @@
         <v>42084</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="140">
         <v>7</v>
       </c>
@@ -10090,7 +10104,7 @@
         <v>42105</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="140">
         <v>10</v>
       </c>
@@ -10134,7 +10148,7 @@
         <v>11856250</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="140">
         <v>11</v>
       </c>
@@ -10332,7 +10346,7 @@
       <c r="M20" s="176"/>
       <c r="N20" s="176"/>
     </row>
-    <row r="21" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="171"/>
       <c r="B21" s="172"/>
       <c r="C21" s="171"/>
@@ -10374,7 +10388,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="171"/>
       <c r="B23" s="172"/>
       <c r="C23" s="171"/>
@@ -10395,7 +10409,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="171"/>
       <c r="B24" s="172"/>
       <c r="C24" s="171"/>
@@ -10416,7 +10430,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="171"/>
       <c r="B25" s="172"/>
       <c r="C25" s="171"/>
@@ -10597,7 +10611,7 @@
       <c r="M35" s="176"/>
       <c r="N35" s="176"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="171"/>
       <c r="B36" s="171"/>
       <c r="C36" s="171"/>
@@ -10613,7 +10627,7 @@
       <c r="M36" s="176"/>
       <c r="N36" s="176"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="171"/>
       <c r="B37" s="171"/>
       <c r="C37" s="171"/>
@@ -10629,7 +10643,7 @@
       <c r="M37" s="176"/>
       <c r="N37" s="176"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="171"/>
       <c r="B38" s="171"/>
       <c r="C38" s="171"/>
@@ -10645,7 +10659,7 @@
       <c r="M38" s="176"/>
       <c r="N38" s="176"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="171"/>
       <c r="B39" s="171"/>
       <c r="C39" s="171"/>
@@ -10661,7 +10675,7 @@
       <c r="M39" s="176"/>
       <c r="N39" s="176"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="171"/>
       <c r="B40" s="171"/>
       <c r="C40" s="171"/>
@@ -10677,127 +10691,127 @@
       <c r="M40" s="176"/>
       <c r="N40" s="176"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="171"/>
       <c r="N41" s="176"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="171"/>
       <c r="N42" s="176"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" s="171"/>
       <c r="N43" s="176"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" s="171"/>
       <c r="N44" s="176"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" s="171"/>
       <c r="N45" s="176"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" s="171"/>
       <c r="N46" s="176"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" s="171"/>
       <c r="N47" s="176"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" s="171"/>
       <c r="N48" s="176"/>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" s="171"/>
       <c r="N49" s="176"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" s="171"/>
       <c r="N50" s="176"/>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" s="171"/>
       <c r="N51" s="176"/>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" s="171"/>
       <c r="N52" s="176"/>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" s="171"/>
       <c r="N53" s="176"/>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54" s="171"/>
       <c r="N54" s="176"/>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" s="171"/>
       <c r="N55" s="176"/>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" s="171"/>
       <c r="N56" s="176"/>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" s="171"/>
       <c r="N57" s="176"/>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58" s="171"/>
       <c r="N58" s="176"/>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59" s="171"/>
       <c r="N59" s="176"/>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60" s="171"/>
       <c r="N60" s="176"/>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61" s="171"/>
       <c r="N61" s="176"/>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62" s="171"/>
       <c r="N62" s="176"/>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63" s="171"/>
       <c r="N63" s="176"/>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A64" s="171"/>
       <c r="N64" s="176"/>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A65" s="171"/>
       <c r="N65" s="176"/>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A66" s="171"/>
       <c r="N66" s="176"/>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67" s="171"/>
       <c r="N67" s="176"/>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A68" s="171"/>
       <c r="N68" s="176"/>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A69" s="171"/>
       <c r="N69" s="176"/>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A70" s="171"/>
       <c r="N70" s="176"/>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A71" s="171"/>
       <c r="N71" s="176"/>
     </row>

</xml_diff>

<commit_message>
V0.6 de SRS V1.4 de SPMP
</commit_message>
<xml_diff>
--- a/Proyecto/Tercer Incremento - Segunda Entrega/Documentos/(SnoutPoint) - Asignación de Recursos y Tiempo.xlsx
+++ b/Proyecto/Tercer Incremento - Segunda Entrega/Documentos/(SnoutPoint) - Asignación de Recursos y Tiempo.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="48" windowWidth="20736" windowHeight="9552" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="20730" windowHeight="9555" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1° Inc - Recursos y Costos" sheetId="1" r:id="rId1"/>
@@ -739,8 +739,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
     <numFmt numFmtId="166" formatCode="_-[$$-240A]\ * #,##0.00_ ;_-[$$-240A]\ * \-#,##0.00\ ;_-[$$-240A]\ * &quot;-&quot;??_ ;_-@_ "/>
     <numFmt numFmtId="167" formatCode="[$-C0A]d\-mmm\-yyyy;@"/>
@@ -1259,8 +1259,8 @@
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="225">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1899,16 +1899,16 @@
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2256,45 +2256,45 @@
       <selection pane="bottomRight" activeCell="K63" sqref="K63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="16" style="1" customWidth="1"/>
-    <col min="8" max="9" width="18.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="29" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.44140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="62.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="62.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="31" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="11.5546875" style="1"/>
+    <col min="19" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="215" t="s">
+    <row r="1" spans="1:18" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="214" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="216"/>
-      <c r="C1" s="216"/>
-      <c r="D1" s="216"/>
-      <c r="E1" s="216"/>
-      <c r="F1" s="216"/>
-      <c r="G1" s="216"/>
-      <c r="H1" s="216"/>
-      <c r="I1" s="216"/>
-      <c r="J1" s="216"/>
-      <c r="K1" s="216"/>
-      <c r="L1" s="217"/>
-    </row>
-    <row r="2" spans="1:18" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="215"/>
+      <c r="C1" s="215"/>
+      <c r="D1" s="215"/>
+      <c r="E1" s="215"/>
+      <c r="F1" s="215"/>
+      <c r="G1" s="215"/>
+      <c r="H1" s="215"/>
+      <c r="I1" s="215"/>
+      <c r="J1" s="215"/>
+      <c r="K1" s="215"/>
+      <c r="L1" s="216"/>
+    </row>
+    <row r="2" spans="1:18" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="83" t="s">
         <v>0</v>
       </c>
@@ -2389,7 +2389,7 @@
       <c r="Q3" s="6"/>
       <c r="R3" s="5"/>
     </row>
-    <row r="4" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="189">
         <v>2</v>
       </c>
@@ -2434,7 +2434,7 @@
       <c r="Q4" s="8"/>
       <c r="R4" s="7"/>
     </row>
-    <row r="5" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="32">
         <v>3</v>
       </c>
@@ -2479,7 +2479,7 @@
       <c r="Q5" s="10"/>
       <c r="R5" s="7"/>
     </row>
-    <row r="6" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="32">
         <v>4</v>
       </c>
@@ -2524,7 +2524,7 @@
       <c r="Q6" s="11"/>
       <c r="R6" s="12"/>
     </row>
-    <row r="7" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="32">
         <v>5</v>
       </c>
@@ -2563,7 +2563,7 @@
       <c r="Q7" s="13"/>
       <c r="R7" s="14"/>
     </row>
-    <row r="8" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="32">
         <v>6</v>
       </c>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="M8" s="44"/>
     </row>
-    <row r="9" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="32">
         <v>7</v>
       </c>
@@ -2638,7 +2638,7 @@
         <v>3528.6458333333335</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="32">
         <v>8</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>3528.6458333333335</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="32">
         <v>9</v>
       </c>
@@ -2712,7 +2712,7 @@
         <v>3528.6458333333335</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A12" s="32">
         <v>10</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>3528.6458333333335</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="32">
         <v>11</v>
       </c>
@@ -2786,7 +2786,7 @@
         <v>3528.6458333333335</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="32">
         <v>12</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>3528.6458333333335</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="32">
         <v>13</v>
       </c>
@@ -2860,7 +2860,7 @@
         <v>3528.6458333333335</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="32">
         <v>14</v>
       </c>
@@ -3136,7 +3136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11">
         <v>22</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>1764.3229166666667</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
         <v>23</v>
       </c>
@@ -3212,7 +3212,7 @@
         <v>7057.291666666667</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="22">
         <v>24</v>
       </c>
@@ -3378,7 +3378,7 @@
         <v>7057.291666666667</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
         <v>29</v>
       </c>
@@ -3412,7 +3412,7 @@
         <v>28229.166666666668</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11">
         <v>30</v>
       </c>
@@ -3542,7 +3542,7 @@
         <v>232890.625</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="22">
         <v>34</v>
       </c>
@@ -3582,7 +3582,7 @@
         <v>105859.375</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="22">
         <v>35</v>
       </c>
@@ -3660,7 +3660,7 @@
         <v>10585.9375</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="22">
         <v>37</v>
       </c>
@@ -3693,14 +3693,14 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O39" s="214" t="s">
+      <c r="O39" s="217" t="s">
         <v>115</v>
       </c>
-      <c r="P39" s="214"/>
-      <c r="Q39" s="214" t="s">
+      <c r="P39" s="217"/>
+      <c r="Q39" s="217" t="s">
         <v>116</v>
       </c>
-      <c r="R39" s="214"/>
+      <c r="R39" s="217"/>
     </row>
     <row r="40" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="22">
@@ -3741,12 +3741,12 @@
       <c r="P40" s="46">
         <v>42042</v>
       </c>
-      <c r="Q40" s="214">
+      <c r="Q40" s="217">
         <v>1</v>
       </c>
-      <c r="R40" s="214"/>
-    </row>
-    <row r="41" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R40" s="217"/>
+    </row>
+    <row r="41" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="22">
         <v>39</v>
       </c>
@@ -3785,12 +3785,12 @@
       <c r="P41" s="46">
         <v>42049</v>
       </c>
-      <c r="Q41" s="214">
+      <c r="Q41" s="217">
         <v>2</v>
       </c>
-      <c r="R41" s="214"/>
-    </row>
-    <row r="42" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R41" s="217"/>
+    </row>
+    <row r="42" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="11">
         <v>40</v>
       </c>
@@ -3833,12 +3833,12 @@
       <c r="P42" s="46">
         <v>42056</v>
       </c>
-      <c r="Q42" s="214">
+      <c r="Q42" s="217">
         <v>3</v>
       </c>
-      <c r="R42" s="214"/>
-    </row>
-    <row r="43" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R42" s="217"/>
+    </row>
+    <row r="43" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
         <v>41</v>
       </c>
@@ -3871,10 +3871,10 @@
       <c r="P43" s="46">
         <v>42063</v>
       </c>
-      <c r="Q43" s="214">
+      <c r="Q43" s="217">
         <v>4</v>
       </c>
-      <c r="R43" s="214"/>
+      <c r="R43" s="217"/>
     </row>
     <row r="44" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="22">
@@ -3921,12 +3921,12 @@
       <c r="P44" s="46">
         <v>42070</v>
       </c>
-      <c r="Q44" s="214">
+      <c r="Q44" s="217">
         <v>5</v>
       </c>
-      <c r="R44" s="214"/>
-    </row>
-    <row r="45" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R44" s="217"/>
+    </row>
+    <row r="45" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="22">
         <v>43</v>
       </c>
@@ -3971,12 +3971,12 @@
       <c r="P45" s="46">
         <v>42077</v>
       </c>
-      <c r="Q45" s="214">
+      <c r="Q45" s="217">
         <v>6</v>
       </c>
-      <c r="R45" s="214"/>
-    </row>
-    <row r="46" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R45" s="217"/>
+    </row>
+    <row r="46" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10">
         <v>44</v>
       </c>
@@ -4005,12 +4005,12 @@
       <c r="P46" s="46">
         <v>42084</v>
       </c>
-      <c r="Q46" s="214">
+      <c r="Q46" s="217">
         <v>7</v>
       </c>
-      <c r="R46" s="214"/>
-    </row>
-    <row r="47" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R46" s="217"/>
+    </row>
+    <row r="47" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="11">
         <v>45</v>
       </c>
@@ -4055,10 +4055,10 @@
       <c r="P47" s="46">
         <v>42091</v>
       </c>
-      <c r="Q47" s="214">
+      <c r="Q47" s="217">
         <v>8</v>
       </c>
-      <c r="R47" s="214"/>
+      <c r="R47" s="217"/>
     </row>
     <row r="48" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="11">
@@ -4095,10 +4095,10 @@
       <c r="P48" s="46">
         <v>42098</v>
       </c>
-      <c r="Q48" s="214">
+      <c r="Q48" s="217">
         <v>9</v>
       </c>
-      <c r="R48" s="214"/>
+      <c r="R48" s="217"/>
     </row>
     <row r="49" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="22">
@@ -4145,10 +4145,10 @@
       <c r="P49" s="46">
         <v>42105</v>
       </c>
-      <c r="Q49" s="214">
+      <c r="Q49" s="217">
         <v>10</v>
       </c>
-      <c r="R49" s="214"/>
+      <c r="R49" s="217"/>
     </row>
     <row r="50" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="22">
@@ -4195,10 +4195,10 @@
       <c r="P50" s="46">
         <v>42112</v>
       </c>
-      <c r="Q50" s="214">
+      <c r="Q50" s="217">
         <v>11</v>
       </c>
-      <c r="R50" s="214"/>
+      <c r="R50" s="217"/>
     </row>
     <row r="51" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="11">
@@ -4231,12 +4231,12 @@
       <c r="P51" s="46">
         <v>42119</v>
       </c>
-      <c r="Q51" s="214">
+      <c r="Q51" s="217">
         <v>12</v>
       </c>
-      <c r="R51" s="214"/>
-    </row>
-    <row r="52" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R51" s="217"/>
+    </row>
+    <row r="52" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="22">
         <v>50</v>
       </c>
@@ -4281,12 +4281,12 @@
       <c r="P52" s="46">
         <v>42126</v>
       </c>
-      <c r="Q52" s="214">
+      <c r="Q52" s="217">
         <v>13</v>
       </c>
-      <c r="R52" s="214"/>
-    </row>
-    <row r="53" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R52" s="217"/>
+    </row>
+    <row r="53" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="22">
         <v>51</v>
       </c>
@@ -4331,12 +4331,12 @@
       <c r="P53" s="46">
         <v>42133</v>
       </c>
-      <c r="Q53" s="214">
+      <c r="Q53" s="217">
         <v>14</v>
       </c>
-      <c r="R53" s="214"/>
-    </row>
-    <row r="54" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R53" s="217"/>
+    </row>
+    <row r="54" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="22">
         <v>52</v>
       </c>
@@ -4381,12 +4381,12 @@
       <c r="P54" s="46">
         <v>42140</v>
       </c>
-      <c r="Q54" s="214">
+      <c r="Q54" s="217">
         <v>15</v>
       </c>
-      <c r="R54" s="214"/>
-    </row>
-    <row r="55" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R54" s="217"/>
+    </row>
+    <row r="55" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="22">
         <v>53</v>
       </c>
@@ -4431,10 +4431,10 @@
       <c r="P55" s="46">
         <v>42147</v>
       </c>
-      <c r="Q55" s="214">
+      <c r="Q55" s="217">
         <v>16</v>
       </c>
-      <c r="R55" s="214"/>
+      <c r="R55" s="217"/>
     </row>
     <row r="56" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="10">
@@ -4465,10 +4465,10 @@
       <c r="P56" s="46">
         <v>42154</v>
       </c>
-      <c r="Q56" s="214">
+      <c r="Q56" s="217">
         <v>17</v>
       </c>
-      <c r="R56" s="214"/>
+      <c r="R56" s="217"/>
     </row>
     <row r="57" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="11">
@@ -4680,7 +4680,7 @@
         <v>7057.291666666667</v>
       </c>
     </row>
-    <row r="62" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="11">
         <v>60</v>
       </c>
@@ -4720,7 +4720,7 @@
         <v>42343.75</v>
       </c>
     </row>
-    <row r="63" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
         <v>61</v>
       </c>
@@ -4760,7 +4760,7 @@
         <v>70572.916666666672</v>
       </c>
     </row>
-    <row r="64" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="11">
         <v>62</v>
       </c>
@@ -4929,26 +4929,26 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="Q52:R52"/>
+    <mergeCell ref="Q53:R53"/>
+    <mergeCell ref="Q54:R54"/>
+    <mergeCell ref="Q55:R55"/>
+    <mergeCell ref="Q56:R56"/>
+    <mergeCell ref="Q47:R47"/>
+    <mergeCell ref="Q48:R48"/>
+    <mergeCell ref="Q49:R49"/>
+    <mergeCell ref="Q50:R50"/>
+    <mergeCell ref="Q51:R51"/>
+    <mergeCell ref="Q42:R42"/>
+    <mergeCell ref="Q43:R43"/>
+    <mergeCell ref="Q44:R44"/>
+    <mergeCell ref="Q45:R45"/>
+    <mergeCell ref="Q46:R46"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="Q40:R40"/>
     <mergeCell ref="O39:P39"/>
     <mergeCell ref="Q39:R39"/>
     <mergeCell ref="Q41:R41"/>
-    <mergeCell ref="Q42:R42"/>
-    <mergeCell ref="Q43:R43"/>
-    <mergeCell ref="Q44:R44"/>
-    <mergeCell ref="Q45:R45"/>
-    <mergeCell ref="Q46:R46"/>
-    <mergeCell ref="Q47:R47"/>
-    <mergeCell ref="Q48:R48"/>
-    <mergeCell ref="Q49:R49"/>
-    <mergeCell ref="Q50:R50"/>
-    <mergeCell ref="Q51:R51"/>
-    <mergeCell ref="Q52:R52"/>
-    <mergeCell ref="Q53:R53"/>
-    <mergeCell ref="Q54:R54"/>
-    <mergeCell ref="Q55:R55"/>
-    <mergeCell ref="Q56:R56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -4963,30 +4963,30 @@
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="19.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="17.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5546875" style="50" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="64.33203125" style="50" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" style="50" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.109375" style="50" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.109375" style="50" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" style="50" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" style="50" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.28515625" style="50" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" style="50" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" style="50" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" style="50" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" style="50" customWidth="1"/>
     <col min="7" max="7" width="16" style="50" customWidth="1"/>
-    <col min="8" max="8" width="16.88671875" style="50" customWidth="1"/>
-    <col min="9" max="9" width="16.44140625" style="50" customWidth="1"/>
-    <col min="10" max="10" width="32.33203125" style="50" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="47.44140625" style="50" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.44140625" style="50" customWidth="1"/>
-    <col min="13" max="13" width="13.88671875" style="50" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.44140625" style="50" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="62.44140625" style="50" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.6640625" style="50" customWidth="1"/>
-    <col min="17" max="17" width="9.6640625" style="50" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" style="50" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" style="50" customWidth="1"/>
+    <col min="10" max="10" width="32.28515625" style="50" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="47.42578125" style="50" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.42578125" style="50" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" style="50" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" style="50" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="62.42578125" style="50" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" style="50" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" style="50" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="31" style="50" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="11.5546875" style="50"/>
+    <col min="19" max="16384" width="11.5703125" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="218" t="s">
         <v>113</v>
       </c>
@@ -5002,7 +5002,7 @@
       <c r="K1" s="219"/>
       <c r="L1" s="220"/>
     </row>
-    <row r="2" spans="1:18" ht="77.400000000000006" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" ht="69.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="79" t="s">
         <v>0</v>
       </c>
@@ -5046,7 +5046,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="51">
         <v>1</v>
       </c>
@@ -5094,7 +5094,7 @@
       <c r="Q3" s="54"/>
       <c r="R3" s="55"/>
     </row>
-    <row r="4" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="61">
         <v>2</v>
       </c>
@@ -5142,7 +5142,7 @@
       <c r="Q4" s="59"/>
       <c r="R4" s="60"/>
     </row>
-    <row r="5" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="87">
         <v>3</v>
       </c>
@@ -5223,7 +5223,7 @@
       <c r="Q6" s="64"/>
       <c r="R6" s="65"/>
     </row>
-    <row r="7" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="87">
         <v>5</v>
       </c>
@@ -5265,7 +5265,7 @@
       <c r="Q7" s="66"/>
       <c r="R7" s="67"/>
     </row>
-    <row r="8" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="87">
         <v>6</v>
       </c>
@@ -5312,7 +5312,7 @@
         <v>42084</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="87">
         <v>7</v>
       </c>
@@ -5389,7 +5389,7 @@
         <v>42098</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="87">
         <v>9</v>
       </c>
@@ -5465,7 +5465,7 @@
         <v>42112</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="38.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="38.450000000000003" x14ac:dyDescent="0.3">
       <c r="A13" s="87">
         <v>11</v>
       </c>
@@ -5511,7 +5511,7 @@
         <v>42119</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="38.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A14" s="87">
         <v>12</v>
       </c>
@@ -5550,7 +5550,7 @@
         <v>42126</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="117">
         <v>13</v>
       </c>
@@ -5589,7 +5589,7 @@
         <v>42133</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="117">
         <v>14</v>
       </c>
@@ -5628,7 +5628,7 @@
         <v>42140</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="97"/>
       <c r="B17" s="91"/>
       <c r="C17" s="91"/>
@@ -5659,7 +5659,7 @@
         <v>42147</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="97"/>
       <c r="B18" s="91"/>
       <c r="C18" s="92"/>
@@ -5679,7 +5679,7 @@
         <v>42154</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="97"/>
       <c r="B19" s="91"/>
       <c r="C19" s="92"/>
@@ -5707,7 +5707,7 @@
       <c r="K20" s="92"/>
       <c r="L20" s="94"/>
     </row>
-    <row r="21" spans="1:15" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="97"/>
       <c r="B21" s="96"/>
       <c r="C21" s="92"/>
@@ -5727,7 +5727,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="97"/>
       <c r="B22" s="209"/>
       <c r="C22" s="92"/>
@@ -5748,7 +5748,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="38.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A23" s="92"/>
       <c r="B23" s="96"/>
       <c r="C23" s="92"/>
@@ -5769,7 +5769,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="92"/>
       <c r="B24" s="96"/>
       <c r="C24" s="92"/>
@@ -5790,7 +5790,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="97"/>
       <c r="B25" s="211"/>
       <c r="C25" s="91"/>
@@ -5811,7 +5811,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="97"/>
       <c r="B26" s="213"/>
       <c r="C26" s="92"/>
@@ -5826,7 +5826,7 @@
       <c r="L26" s="212"/>
       <c r="M26" s="91"/>
     </row>
-    <row r="27" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="97"/>
       <c r="B27" s="213"/>
       <c r="C27" s="92"/>
@@ -5841,7 +5841,7 @@
       <c r="L27" s="212"/>
       <c r="M27" s="91"/>
     </row>
-    <row r="28" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="92"/>
       <c r="B28" s="96"/>
       <c r="C28" s="92"/>
@@ -5856,7 +5856,7 @@
       <c r="L28" s="94"/>
       <c r="M28" s="91"/>
     </row>
-    <row r="29" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="92"/>
       <c r="B29" s="96"/>
       <c r="C29" s="92"/>
@@ -5871,7 +5871,7 @@
       <c r="L29" s="94"/>
       <c r="M29" s="91"/>
     </row>
-    <row r="30" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="92"/>
       <c r="B30" s="96"/>
       <c r="C30" s="92"/>
@@ -5886,7 +5886,7 @@
       <c r="L30" s="94"/>
       <c r="M30" s="91"/>
     </row>
-    <row r="31" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="92"/>
       <c r="B31" s="96"/>
       <c r="C31" s="92"/>
@@ -5900,7 +5900,7 @@
       <c r="K31" s="92"/>
       <c r="L31" s="94"/>
     </row>
-    <row r="32" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="92"/>
       <c r="B32" s="96"/>
       <c r="C32" s="92"/>
@@ -5914,7 +5914,7 @@
       <c r="K32" s="92"/>
       <c r="L32" s="94"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="92"/>
       <c r="B33" s="96"/>
       <c r="C33" s="92"/>
@@ -5928,7 +5928,7 @@
       <c r="K33" s="92"/>
       <c r="L33" s="94"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="92"/>
       <c r="B34" s="96"/>
       <c r="C34" s="92"/>
@@ -5942,7 +5942,7 @@
       <c r="K34" s="92"/>
       <c r="L34" s="94"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="92"/>
       <c r="B35" s="95"/>
       <c r="C35" s="92"/>
@@ -5956,7 +5956,7 @@
       <c r="K35" s="92"/>
       <c r="L35" s="94"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="92"/>
       <c r="B36" s="96"/>
       <c r="C36" s="92"/>
@@ -5970,7 +5970,7 @@
       <c r="K36" s="92"/>
       <c r="L36" s="94"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="92"/>
       <c r="B37" s="96"/>
       <c r="C37" s="92"/>
@@ -5984,7 +5984,7 @@
       <c r="K37" s="92"/>
       <c r="L37" s="94"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="92"/>
       <c r="B38" s="96"/>
       <c r="C38" s="92"/>
@@ -5998,7 +5998,7 @@
       <c r="K38" s="92"/>
       <c r="L38" s="94"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="92"/>
       <c r="B39" s="96"/>
       <c r="C39" s="92"/>
@@ -6012,7 +6012,7 @@
       <c r="K39" s="92"/>
       <c r="L39" s="94"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="92"/>
       <c r="B40" s="96"/>
       <c r="C40" s="92"/>
@@ -6026,7 +6026,7 @@
       <c r="K40" s="92"/>
       <c r="L40" s="94"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="92"/>
       <c r="B41" s="96"/>
       <c r="C41" s="92"/>
@@ -6040,7 +6040,7 @@
       <c r="K41" s="92"/>
       <c r="L41" s="94"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="92"/>
       <c r="B42" s="96"/>
       <c r="C42" s="92"/>
@@ -6054,7 +6054,7 @@
       <c r="K42" s="92"/>
       <c r="L42" s="94"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="92"/>
       <c r="B43" s="96"/>
       <c r="C43" s="92"/>
@@ -6068,7 +6068,7 @@
       <c r="K43" s="92"/>
       <c r="L43" s="94"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="92"/>
       <c r="B44" s="96"/>
       <c r="C44" s="92"/>
@@ -6082,7 +6082,7 @@
       <c r="K44" s="92"/>
       <c r="L44" s="94"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="92"/>
       <c r="B45" s="96"/>
       <c r="C45" s="92"/>
@@ -6096,7 +6096,7 @@
       <c r="K45" s="92"/>
       <c r="L45" s="94"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="92"/>
       <c r="B46" s="96"/>
       <c r="C46" s="92"/>
@@ -6110,7 +6110,7 @@
       <c r="K46" s="92"/>
       <c r="L46" s="94"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="92"/>
       <c r="B47" s="96"/>
       <c r="C47" s="92"/>
@@ -6124,7 +6124,7 @@
       <c r="K47" s="92"/>
       <c r="L47" s="94"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="92"/>
       <c r="B48" s="95"/>
       <c r="C48" s="92"/>
@@ -6138,7 +6138,7 @@
       <c r="K48" s="92"/>
       <c r="L48" s="94"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="92"/>
       <c r="B49" s="96"/>
       <c r="C49" s="92"/>
@@ -6152,7 +6152,7 @@
       <c r="K49" s="92"/>
       <c r="L49" s="94"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="92"/>
       <c r="B50" s="96"/>
       <c r="C50" s="92"/>
@@ -6166,7 +6166,7 @@
       <c r="K50" s="92"/>
       <c r="L50" s="94"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="92"/>
       <c r="B51" s="96"/>
       <c r="C51" s="92"/>
@@ -6180,7 +6180,7 @@
       <c r="K51" s="92"/>
       <c r="L51" s="94"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="92"/>
       <c r="B52" s="96"/>
       <c r="C52" s="92"/>
@@ -6194,7 +6194,7 @@
       <c r="K52" s="92"/>
       <c r="L52" s="94"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="92"/>
       <c r="B53" s="96"/>
       <c r="C53" s="92"/>
@@ -6208,7 +6208,7 @@
       <c r="K53" s="92"/>
       <c r="L53" s="94"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="92"/>
       <c r="B54" s="96"/>
       <c r="C54" s="92"/>
@@ -6222,7 +6222,7 @@
       <c r="K54" s="92"/>
       <c r="L54" s="94"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="92"/>
       <c r="B55" s="96"/>
       <c r="C55" s="92"/>
@@ -6236,7 +6236,7 @@
       <c r="K55" s="92"/>
       <c r="L55" s="94"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="92"/>
       <c r="B56" s="96"/>
       <c r="C56" s="92"/>
@@ -6250,7 +6250,7 @@
       <c r="K56" s="92"/>
       <c r="L56" s="94"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="92"/>
       <c r="B57" s="96"/>
       <c r="C57" s="92"/>
@@ -6264,7 +6264,7 @@
       <c r="K57" s="92"/>
       <c r="L57" s="94"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="92"/>
       <c r="B58" s="96"/>
       <c r="C58" s="92"/>
@@ -6278,7 +6278,7 @@
       <c r="K58" s="92"/>
       <c r="L58" s="94"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="92"/>
       <c r="B59" s="96"/>
       <c r="C59" s="92"/>
@@ -6292,7 +6292,7 @@
       <c r="K59" s="92"/>
       <c r="L59" s="94"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="92"/>
       <c r="B60" s="96"/>
       <c r="C60" s="92"/>
@@ -6306,7 +6306,7 @@
       <c r="K60" s="92"/>
       <c r="L60" s="94"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="92"/>
       <c r="B61" s="92"/>
       <c r="C61" s="92"/>
@@ -6320,7 +6320,7 @@
       <c r="K61" s="92"/>
       <c r="L61" s="94"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="92"/>
       <c r="B62" s="92"/>
       <c r="C62" s="92"/>
@@ -6334,7 +6334,7 @@
       <c r="K62" s="92"/>
       <c r="L62" s="94"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="92"/>
       <c r="B63" s="92"/>
       <c r="C63" s="92"/>
@@ -6348,7 +6348,7 @@
       <c r="K63" s="92"/>
       <c r="L63" s="94"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="92"/>
       <c r="B64" s="92"/>
       <c r="C64" s="92"/>
@@ -6362,7 +6362,7 @@
       <c r="K64" s="92"/>
       <c r="L64" s="94"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="92"/>
       <c r="B65" s="92"/>
       <c r="C65" s="92"/>
@@ -6376,7 +6376,7 @@
       <c r="K65" s="92"/>
       <c r="L65" s="94"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="92"/>
       <c r="B66" s="92"/>
       <c r="C66" s="92"/>
@@ -6390,7 +6390,7 @@
       <c r="K66" s="92"/>
       <c r="L66" s="94"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="92"/>
       <c r="B67" s="92"/>
       <c r="C67" s="92"/>
@@ -6404,19 +6404,19 @@
       <c r="K67" s="92"/>
       <c r="L67" s="94"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="92"/>
       <c r="B68" s="91"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="91"/>
       <c r="B69" s="91"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="91"/>
       <c r="B70" s="91"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="91"/>
       <c r="B71" s="91"/>
     </row>
@@ -6437,28 +6437,28 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="19.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="17.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5546875" style="50" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.109375" style="50" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" style="50" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" style="50" customWidth="1"/>
-    <col min="5" max="6" width="16.5546875" style="50" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" style="50" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.140625" style="50" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="50" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="50" customWidth="1"/>
+    <col min="5" max="6" width="16.5703125" style="50" customWidth="1"/>
     <col min="7" max="7" width="16" style="50" customWidth="1"/>
-    <col min="8" max="9" width="18.44140625" style="50" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="18.42578125" style="50" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="29" style="50" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="57.33203125" style="50" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.44140625" style="50" customWidth="1"/>
-    <col min="13" max="13" width="13.88671875" style="50" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.44140625" style="50" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="62.44140625" style="50" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.6640625" style="50" customWidth="1"/>
-    <col min="17" max="17" width="9.6640625" style="50" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="57.28515625" style="50" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.42578125" style="50" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" style="50" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" style="50" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="62.42578125" style="50" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" style="50" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" style="50" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="31" style="50" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="11.5546875" style="50"/>
+    <col min="19" max="16384" width="11.5703125" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="221" t="s">
         <v>113</v>
       </c>
@@ -6474,7 +6474,7 @@
       <c r="K1" s="221"/>
       <c r="L1" s="221"/>
     </row>
-    <row r="2" spans="1:18" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="116" t="s">
         <v>0</v>
       </c>
@@ -6518,7 +6518,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="51">
         <v>1</v>
       </c>
@@ -6583,7 +6583,7 @@
       <c r="Q4" s="59"/>
       <c r="R4" s="60"/>
     </row>
-    <row r="5" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="87">
         <v>3</v>
       </c>
@@ -6632,7 +6632,7 @@
       <c r="Q5" s="63"/>
       <c r="R5" s="60"/>
     </row>
-    <row r="6" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="87">
         <v>4</v>
       </c>
@@ -6725,7 +6725,7 @@
       <c r="Q7" s="201"/>
       <c r="R7" s="202"/>
     </row>
-    <row r="8" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="61">
         <v>6</v>
       </c>
@@ -6769,7 +6769,7 @@
       <c r="Q8" s="201"/>
       <c r="R8" s="202"/>
     </row>
-    <row r="9" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="87">
         <v>7</v>
       </c>
@@ -6999,7 +6999,7 @@
         <v>42112</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="51">
         <v>13</v>
       </c>
@@ -7038,7 +7038,7 @@
         <v>42119</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="61">
         <v>14</v>
       </c>
@@ -7122,7 +7122,7 @@
         <v>42133</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="117">
         <v>16</v>
       </c>
@@ -7161,7 +7161,7 @@
         <v>42140</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="97"/>
       <c r="F19" s="50">
         <f>SUM(F3:F18)</f>
@@ -7186,7 +7186,7 @@
         <v>42147</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="97"/>
       <c r="B20" s="125"/>
       <c r="C20" s="97"/>
@@ -7207,7 +7207,7 @@
         <v>42154</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="97"/>
       <c r="B21" s="125"/>
       <c r="C21" s="97"/>
@@ -7241,7 +7241,7 @@
       <c r="N22" s="101"/>
       <c r="O22" s="101"/>
     </row>
-    <row r="23" spans="1:15" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="97"/>
       <c r="B23" s="125"/>
       <c r="C23" s="97"/>
@@ -7262,7 +7262,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="97"/>
       <c r="B24" s="125"/>
       <c r="C24" s="97"/>
@@ -7283,7 +7283,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="38.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A25" s="97"/>
       <c r="B25" s="125"/>
       <c r="C25" s="97"/>
@@ -7304,7 +7304,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="97"/>
       <c r="B26" s="125"/>
       <c r="C26" s="97"/>
@@ -7325,7 +7325,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="97"/>
       <c r="B27" s="125"/>
       <c r="C27" s="97"/>
@@ -7346,7 +7346,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="97"/>
       <c r="B28" s="125"/>
       <c r="C28" s="97"/>
@@ -7363,7 +7363,7 @@
       <c r="N28" s="101"/>
       <c r="O28" s="101"/>
     </row>
-    <row r="29" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="97"/>
       <c r="B29" s="125"/>
       <c r="C29" s="97"/>
@@ -7380,7 +7380,7 @@
       <c r="N29" s="101"/>
       <c r="O29" s="101"/>
     </row>
-    <row r="30" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="97"/>
       <c r="B30" s="125"/>
       <c r="C30" s="97"/>
@@ -7397,7 +7397,7 @@
       <c r="N30" s="101"/>
       <c r="O30" s="101"/>
     </row>
-    <row r="31" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="97"/>
       <c r="B31" s="125"/>
       <c r="C31" s="97"/>
@@ -7414,7 +7414,7 @@
       <c r="N31" s="101"/>
       <c r="O31" s="101"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="97"/>
       <c r="B32" s="125"/>
       <c r="C32" s="97"/>
@@ -7431,7 +7431,7 @@
       <c r="N32" s="101"/>
       <c r="O32" s="101"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="97"/>
       <c r="B33" s="125"/>
       <c r="C33" s="97"/>
@@ -7448,7 +7448,7 @@
       <c r="N33" s="101"/>
       <c r="O33" s="101"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="97"/>
       <c r="B34" s="125"/>
       <c r="C34" s="97"/>
@@ -7465,7 +7465,7 @@
       <c r="N34" s="101"/>
       <c r="O34" s="101"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="97"/>
       <c r="B35" s="125"/>
       <c r="C35" s="97"/>
@@ -7482,7 +7482,7 @@
       <c r="N35" s="101"/>
       <c r="O35" s="101"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="97"/>
       <c r="B36" s="125"/>
       <c r="C36" s="97"/>
@@ -7499,7 +7499,7 @@
       <c r="N36" s="101"/>
       <c r="O36" s="101"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="97"/>
       <c r="B37" s="125"/>
       <c r="C37" s="97"/>
@@ -7516,7 +7516,7 @@
       <c r="N37" s="101"/>
       <c r="O37" s="101"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="97"/>
       <c r="B38" s="125"/>
       <c r="C38" s="97"/>
@@ -7533,7 +7533,7 @@
       <c r="N38" s="101"/>
       <c r="O38" s="101"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="97"/>
       <c r="B39" s="125"/>
       <c r="C39" s="97"/>
@@ -7550,7 +7550,7 @@
       <c r="N39" s="101"/>
       <c r="O39" s="101"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="97"/>
       <c r="B40" s="125"/>
       <c r="C40" s="97"/>
@@ -7567,7 +7567,7 @@
       <c r="N40" s="101"/>
       <c r="O40" s="101"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="97"/>
       <c r="B41" s="125"/>
       <c r="C41" s="97"/>
@@ -7584,7 +7584,7 @@
       <c r="N41" s="101"/>
       <c r="O41" s="101"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="97"/>
       <c r="B42" s="125"/>
       <c r="C42" s="97"/>
@@ -7601,7 +7601,7 @@
       <c r="N42" s="101"/>
       <c r="O42" s="101"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="97"/>
       <c r="B43" s="125"/>
       <c r="C43" s="97"/>
@@ -7618,7 +7618,7 @@
       <c r="N43" s="101"/>
       <c r="O43" s="101"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="97"/>
       <c r="B44" s="125"/>
       <c r="C44" s="97"/>
@@ -7635,7 +7635,7 @@
       <c r="N44" s="101"/>
       <c r="O44" s="101"/>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="97"/>
       <c r="B45" s="125"/>
       <c r="C45" s="97"/>
@@ -7652,7 +7652,7 @@
       <c r="N45" s="101"/>
       <c r="O45" s="101"/>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="97"/>
       <c r="B46" s="125"/>
       <c r="C46" s="97"/>
@@ -7669,7 +7669,7 @@
       <c r="N46" s="101"/>
       <c r="O46" s="101"/>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="97"/>
       <c r="B47" s="125"/>
       <c r="C47" s="97"/>
@@ -7686,7 +7686,7 @@
       <c r="N47" s="101"/>
       <c r="O47" s="101"/>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="97"/>
       <c r="B48" s="125"/>
       <c r="C48" s="97"/>
@@ -7703,7 +7703,7 @@
       <c r="N48" s="101"/>
       <c r="O48" s="101"/>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="97"/>
       <c r="B49" s="125"/>
       <c r="C49" s="97"/>
@@ -7720,7 +7720,7 @@
       <c r="N49" s="101"/>
       <c r="O49" s="101"/>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="97"/>
       <c r="B50" s="125"/>
       <c r="C50" s="97"/>
@@ -7737,7 +7737,7 @@
       <c r="N50" s="101"/>
       <c r="O50" s="101"/>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="97"/>
       <c r="B51" s="125"/>
       <c r="C51" s="97"/>
@@ -7754,7 +7754,7 @@
       <c r="N51" s="101"/>
       <c r="O51" s="101"/>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="97"/>
       <c r="B52" s="125"/>
       <c r="C52" s="97"/>
@@ -7771,7 +7771,7 @@
       <c r="N52" s="101"/>
       <c r="O52" s="101"/>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="97"/>
       <c r="B53" s="125"/>
       <c r="C53" s="97"/>
@@ -7788,7 +7788,7 @@
       <c r="N53" s="101"/>
       <c r="O53" s="101"/>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="97"/>
       <c r="B54" s="125"/>
       <c r="C54" s="97"/>
@@ -7805,7 +7805,7 @@
       <c r="N54" s="101"/>
       <c r="O54" s="101"/>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="97"/>
       <c r="B55" s="125"/>
       <c r="C55" s="97"/>
@@ -7822,7 +7822,7 @@
       <c r="N55" s="101"/>
       <c r="O55" s="101"/>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="97"/>
       <c r="B56" s="125"/>
       <c r="C56" s="97"/>
@@ -7839,7 +7839,7 @@
       <c r="N56" s="101"/>
       <c r="O56" s="101"/>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="97"/>
       <c r="B57" s="125"/>
       <c r="C57" s="97"/>
@@ -7856,7 +7856,7 @@
       <c r="N57" s="101"/>
       <c r="O57" s="101"/>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="97"/>
       <c r="B58" s="125"/>
       <c r="C58" s="97"/>
@@ -7873,7 +7873,7 @@
       <c r="N58" s="101"/>
       <c r="O58" s="101"/>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="97"/>
       <c r="B59" s="125"/>
       <c r="C59" s="97"/>
@@ -7890,7 +7890,7 @@
       <c r="N59" s="101"/>
       <c r="O59" s="101"/>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="97"/>
       <c r="B60" s="125"/>
       <c r="C60" s="97"/>
@@ -7907,7 +7907,7 @@
       <c r="N60" s="101"/>
       <c r="O60" s="101"/>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="97"/>
       <c r="B61" s="125"/>
       <c r="C61" s="97"/>
@@ -7924,7 +7924,7 @@
       <c r="N61" s="101"/>
       <c r="O61" s="101"/>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="97"/>
       <c r="B62" s="125"/>
       <c r="C62" s="97"/>
@@ -7941,7 +7941,7 @@
       <c r="N62" s="101"/>
       <c r="O62" s="101"/>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="97"/>
       <c r="B63" s="97"/>
       <c r="C63" s="97"/>
@@ -7958,7 +7958,7 @@
       <c r="N63" s="101"/>
       <c r="O63" s="101"/>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="97"/>
       <c r="B64" s="97"/>
       <c r="C64" s="97"/>
@@ -7975,7 +7975,7 @@
       <c r="N64" s="101"/>
       <c r="O64" s="101"/>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="97"/>
       <c r="B65" s="97"/>
       <c r="C65" s="97"/>
@@ -7992,7 +7992,7 @@
       <c r="N65" s="101"/>
       <c r="O65" s="101"/>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="97"/>
       <c r="B66" s="97"/>
       <c r="C66" s="97"/>
@@ -8009,7 +8009,7 @@
       <c r="N66" s="101"/>
       <c r="O66" s="101"/>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="97"/>
       <c r="B67" s="97"/>
       <c r="C67" s="97"/>
@@ -8026,7 +8026,7 @@
       <c r="N67" s="101"/>
       <c r="O67" s="101"/>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="97"/>
       <c r="B68" s="97"/>
       <c r="C68" s="97"/>
@@ -8043,7 +8043,7 @@
       <c r="N68" s="101"/>
       <c r="O68" s="101"/>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="97"/>
       <c r="B69" s="97"/>
       <c r="C69" s="97"/>
@@ -8060,7 +8060,7 @@
       <c r="N69" s="101"/>
       <c r="O69" s="101"/>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="97"/>
       <c r="B70" s="97"/>
       <c r="C70" s="97"/>
@@ -8077,7 +8077,7 @@
       <c r="N70" s="101"/>
       <c r="O70" s="101"/>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" s="97"/>
       <c r="B71" s="97"/>
       <c r="C71" s="97"/>
@@ -8094,7 +8094,7 @@
       <c r="N71" s="101"/>
       <c r="O71" s="101"/>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="97"/>
       <c r="B72" s="97"/>
       <c r="C72" s="97"/>
@@ -8111,7 +8111,7 @@
       <c r="N72" s="101"/>
       <c r="O72" s="101"/>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" s="97"/>
       <c r="B73" s="97"/>
       <c r="C73" s="97"/>
@@ -8128,7 +8128,7 @@
       <c r="N73" s="101"/>
       <c r="O73" s="101"/>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="97"/>
       <c r="B74" s="97"/>
       <c r="C74" s="101"/>
@@ -8162,30 +8162,30 @@
       <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="19.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="17.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5546875" style="50" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" style="50" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43" style="50" customWidth="1"/>
-    <col min="3" max="3" width="20.109375" style="50" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="50" customWidth="1"/>
     <col min="4" max="4" width="19" style="50" customWidth="1"/>
     <col min="5" max="5" width="16" style="50" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" style="50" customWidth="1"/>
-    <col min="7" max="7" width="13.88671875" style="50" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" style="50" customWidth="1"/>
-    <col min="9" max="9" width="16.88671875" style="50" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="50" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="50" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" style="50" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" style="50" customWidth="1"/>
     <col min="10" max="10" width="29" style="50" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="57.33203125" style="50" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.44140625" style="50" customWidth="1"/>
-    <col min="13" max="13" width="13.88671875" style="50" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.44140625" style="50" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="62.44140625" style="50" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.6640625" style="50" customWidth="1"/>
-    <col min="17" max="17" width="9.6640625" style="50" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="57.28515625" style="50" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.42578125" style="50" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" style="50" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" style="50" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="62.42578125" style="50" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" style="50" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" style="50" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="31" style="50" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="11.5546875" style="50"/>
+    <col min="19" max="16384" width="11.5703125" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="218" t="s">
         <v>113</v>
       </c>
@@ -8201,7 +8201,7 @@
       <c r="K1" s="219"/>
       <c r="L1" s="220"/>
     </row>
-    <row r="2" spans="1:18" ht="86.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" ht="86.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="79" t="s">
         <v>0</v>
       </c>
@@ -8245,7 +8245,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="51">
         <v>1</v>
       </c>
@@ -8371,7 +8371,7 @@
       <c r="Q5" s="63"/>
       <c r="R5" s="60"/>
     </row>
-    <row r="6" spans="1:18" s="101" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" s="101" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="87">
         <v>4</v>
       </c>
@@ -8525,7 +8525,7 @@
         <v>42084</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="61">
         <v>8</v>
       </c>
@@ -8649,7 +8649,7 @@
         <v>42105</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="61">
         <v>11</v>
       </c>
@@ -8688,7 +8688,7 @@
         <v>42112</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="61">
         <v>12</v>
       </c>
@@ -8727,7 +8727,7 @@
         <v>42119</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="117">
         <v>13</v>
       </c>
@@ -8803,7 +8803,7 @@
         <v>42140</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="97"/>
       <c r="B18" s="108"/>
       <c r="C18" s="97"/>
@@ -8824,7 +8824,7 @@
         <v>42147</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="97"/>
       <c r="B19" s="108"/>
       <c r="C19" s="97"/>
@@ -8845,7 +8845,7 @@
         <v>42154</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="97"/>
       <c r="B20" s="108"/>
       <c r="C20" s="97"/>
@@ -8875,7 +8875,7 @@
       <c r="L21" s="111"/>
       <c r="M21" s="78"/>
     </row>
-    <row r="22" spans="1:15" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="97"/>
       <c r="B22" s="108"/>
       <c r="C22" s="97"/>
@@ -8896,7 +8896,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="97"/>
       <c r="B23" s="108"/>
       <c r="C23" s="97"/>
@@ -8917,7 +8917,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="38.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A24" s="97"/>
       <c r="B24" s="108"/>
       <c r="C24" s="97"/>
@@ -8938,7 +8938,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="97"/>
       <c r="B25" s="108"/>
       <c r="C25" s="97"/>
@@ -8959,7 +8959,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="19.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="97"/>
       <c r="B26" s="108"/>
       <c r="C26" s="97"/>
@@ -8980,7 +8980,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="97"/>
       <c r="B27" s="108"/>
       <c r="C27" s="97"/>
@@ -8995,7 +8995,7 @@
       <c r="L27" s="111"/>
       <c r="M27" s="78"/>
     </row>
-    <row r="28" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="97"/>
       <c r="B28" s="108"/>
       <c r="C28" s="97"/>
@@ -9010,7 +9010,7 @@
       <c r="L28" s="111"/>
       <c r="M28" s="78"/>
     </row>
-    <row r="29" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="97"/>
       <c r="B29" s="108"/>
       <c r="C29" s="97"/>
@@ -9025,7 +9025,7 @@
       <c r="L29" s="111"/>
       <c r="M29" s="78"/>
     </row>
-    <row r="30" spans="1:15" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="97"/>
       <c r="B30" s="108"/>
       <c r="C30" s="97"/>
@@ -9040,7 +9040,7 @@
       <c r="L30" s="111"/>
       <c r="M30" s="78"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="97"/>
       <c r="B31" s="108"/>
       <c r="C31" s="97"/>
@@ -9055,7 +9055,7 @@
       <c r="L31" s="111"/>
       <c r="M31" s="78"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="97"/>
       <c r="B32" s="108"/>
       <c r="C32" s="97"/>
@@ -9070,7 +9070,7 @@
       <c r="L32" s="111"/>
       <c r="M32" s="78"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="97"/>
       <c r="B33" s="108"/>
       <c r="C33" s="97"/>
@@ -9085,7 +9085,7 @@
       <c r="L33" s="111"/>
       <c r="M33" s="78"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="97"/>
       <c r="B34" s="108"/>
       <c r="C34" s="97"/>
@@ -9100,7 +9100,7 @@
       <c r="L34" s="111"/>
       <c r="M34" s="78"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="97"/>
       <c r="B35" s="108"/>
       <c r="C35" s="97"/>
@@ -9115,7 +9115,7 @@
       <c r="L35" s="111"/>
       <c r="M35" s="78"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="97"/>
       <c r="B36" s="112"/>
       <c r="C36" s="97"/>
@@ -9130,7 +9130,7 @@
       <c r="L36" s="111"/>
       <c r="M36" s="78"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="97"/>
       <c r="B37" s="108"/>
       <c r="C37" s="97"/>
@@ -9145,7 +9145,7 @@
       <c r="L37" s="111"/>
       <c r="M37" s="78"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="97"/>
       <c r="B38" s="108"/>
       <c r="C38" s="97"/>
@@ -9160,7 +9160,7 @@
       <c r="L38" s="111"/>
       <c r="M38" s="78"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="97"/>
       <c r="B39" s="108"/>
       <c r="C39" s="97"/>
@@ -9175,7 +9175,7 @@
       <c r="L39" s="111"/>
       <c r="M39" s="78"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="97"/>
       <c r="B40" s="108"/>
       <c r="C40" s="97"/>
@@ -9190,7 +9190,7 @@
       <c r="L40" s="111"/>
       <c r="M40" s="78"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="97"/>
       <c r="B41" s="108"/>
       <c r="C41" s="97"/>
@@ -9205,7 +9205,7 @@
       <c r="L41" s="111"/>
       <c r="M41" s="78"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="97"/>
       <c r="B42" s="108"/>
       <c r="C42" s="97"/>
@@ -9220,7 +9220,7 @@
       <c r="L42" s="111"/>
       <c r="M42" s="78"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="97"/>
       <c r="B43" s="108"/>
       <c r="C43" s="97"/>
@@ -9235,7 +9235,7 @@
       <c r="L43" s="111"/>
       <c r="M43" s="78"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="97"/>
       <c r="B44" s="108"/>
       <c r="C44" s="97"/>
@@ -9250,7 +9250,7 @@
       <c r="L44" s="111"/>
       <c r="M44" s="78"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="97"/>
       <c r="B45" s="108"/>
       <c r="C45" s="97"/>
@@ -9265,7 +9265,7 @@
       <c r="L45" s="111"/>
       <c r="M45" s="78"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="97"/>
       <c r="B46" s="108"/>
       <c r="C46" s="97"/>
@@ -9280,7 +9280,7 @@
       <c r="L46" s="111"/>
       <c r="M46" s="78"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="97"/>
       <c r="B47" s="108"/>
       <c r="C47" s="97"/>
@@ -9295,7 +9295,7 @@
       <c r="L47" s="111"/>
       <c r="M47" s="78"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="97"/>
       <c r="B48" s="108"/>
       <c r="C48" s="97"/>
@@ -9310,7 +9310,7 @@
       <c r="L48" s="111"/>
       <c r="M48" s="78"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="97"/>
       <c r="B49" s="112"/>
       <c r="C49" s="97"/>
@@ -9325,7 +9325,7 @@
       <c r="L49" s="111"/>
       <c r="M49" s="78"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="97"/>
       <c r="B50" s="108"/>
       <c r="C50" s="97"/>
@@ -9340,7 +9340,7 @@
       <c r="L50" s="111"/>
       <c r="M50" s="78"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="97"/>
       <c r="B51" s="108"/>
       <c r="C51" s="97"/>
@@ -9355,7 +9355,7 @@
       <c r="L51" s="111"/>
       <c r="M51" s="78"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="97"/>
       <c r="B52" s="108"/>
       <c r="C52" s="97"/>
@@ -9370,7 +9370,7 @@
       <c r="L52" s="111"/>
       <c r="M52" s="78"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="97"/>
       <c r="B53" s="108"/>
       <c r="C53" s="97"/>
@@ -9385,7 +9385,7 @@
       <c r="L53" s="111"/>
       <c r="M53" s="78"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="97"/>
       <c r="B54" s="108"/>
       <c r="C54" s="97"/>
@@ -9400,7 +9400,7 @@
       <c r="L54" s="111"/>
       <c r="M54" s="78"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="97"/>
       <c r="B55" s="108"/>
       <c r="C55" s="97"/>
@@ -9415,7 +9415,7 @@
       <c r="L55" s="111"/>
       <c r="M55" s="78"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="97"/>
       <c r="B56" s="108"/>
       <c r="C56" s="97"/>
@@ -9430,7 +9430,7 @@
       <c r="L56" s="111"/>
       <c r="M56" s="78"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="97"/>
       <c r="B57" s="108"/>
       <c r="C57" s="97"/>
@@ -9445,7 +9445,7 @@
       <c r="L57" s="111"/>
       <c r="M57" s="78"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="97"/>
       <c r="B58" s="108"/>
       <c r="C58" s="97"/>
@@ -9460,7 +9460,7 @@
       <c r="L58" s="111"/>
       <c r="M58" s="78"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="97"/>
       <c r="B59" s="108"/>
       <c r="C59" s="97"/>
@@ -9475,7 +9475,7 @@
       <c r="L59" s="111"/>
       <c r="M59" s="78"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="97"/>
       <c r="B60" s="108"/>
       <c r="C60" s="97"/>
@@ -9490,7 +9490,7 @@
       <c r="L60" s="111"/>
       <c r="M60" s="78"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="97"/>
       <c r="B61" s="108"/>
       <c r="C61" s="97"/>
@@ -9505,7 +9505,7 @@
       <c r="L61" s="111"/>
       <c r="M61" s="78"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="97"/>
       <c r="B62" s="97"/>
       <c r="C62" s="97"/>
@@ -9520,7 +9520,7 @@
       <c r="L62" s="111"/>
       <c r="M62" s="78"/>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="97"/>
       <c r="B63" s="97"/>
       <c r="C63" s="97"/>
@@ -9535,7 +9535,7 @@
       <c r="L63" s="111"/>
       <c r="M63" s="78"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="97"/>
       <c r="B64" s="97"/>
       <c r="C64" s="97"/>
@@ -9550,7 +9550,7 @@
       <c r="L64" s="111"/>
       <c r="M64" s="78"/>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="97"/>
       <c r="B65" s="97"/>
       <c r="C65" s="97"/>
@@ -9565,7 +9565,7 @@
       <c r="L65" s="111"/>
       <c r="M65" s="78"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="97"/>
       <c r="B66" s="97"/>
       <c r="C66" s="97"/>
@@ -9580,7 +9580,7 @@
       <c r="L66" s="111"/>
       <c r="M66" s="78"/>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="97"/>
       <c r="B67" s="97"/>
       <c r="C67" s="97"/>
@@ -9595,7 +9595,7 @@
       <c r="L67" s="111"/>
       <c r="M67" s="78"/>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="97"/>
       <c r="B68" s="97"/>
       <c r="C68" s="97"/>
@@ -9610,7 +9610,7 @@
       <c r="L68" s="111"/>
       <c r="M68" s="78"/>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="78"/>
       <c r="B69" s="78"/>
       <c r="K69" s="89" t="s">
@@ -9621,11 +9621,11 @@
         <v>1665520.8333333335</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="78"/>
       <c r="B70" s="78"/>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="78"/>
       <c r="B71" s="78"/>
     </row>
@@ -9646,30 +9646,30 @@
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5546875" style="133" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.109375" style="133" customWidth="1"/>
-    <col min="3" max="3" width="21.88671875" style="133" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" style="133" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" style="133" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" style="133" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="133" customWidth="1"/>
-    <col min="8" max="8" width="22.88671875" style="133" customWidth="1"/>
-    <col min="9" max="9" width="18.44140625" style="133" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.5546875" style="133" customWidth="1"/>
-    <col min="11" max="11" width="19.33203125" style="133" customWidth="1"/>
-    <col min="12" max="12" width="26.33203125" style="133" customWidth="1"/>
-    <col min="13" max="13" width="13.88671875" style="133" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.44140625" style="133" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="62.44140625" style="133" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.6640625" style="133" customWidth="1"/>
-    <col min="17" max="17" width="9.6640625" style="133" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" style="133" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" style="133" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" style="133" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" style="133" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" style="133" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" style="133" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="133" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" style="133" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" style="133" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.5703125" style="133" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" style="133" customWidth="1"/>
+    <col min="12" max="12" width="26.28515625" style="133" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" style="133" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" style="133" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="62.42578125" style="133" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" style="133" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" style="133" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="31" style="133" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="11.44140625" style="133"/>
+    <col min="19" max="16384" width="11.42578125" style="133"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="222" t="s">
         <v>113</v>
       </c>
@@ -9685,7 +9685,7 @@
       <c r="K1" s="223"/>
       <c r="L1" s="224"/>
     </row>
-    <row r="2" spans="1:18" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="134" t="s">
         <v>0</v>
       </c>
@@ -9729,7 +9729,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="138">
         <v>1</v>
       </c>
@@ -9858,7 +9858,7 @@
       <c r="Q5" s="157"/>
       <c r="R5" s="154"/>
     </row>
-    <row r="6" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="140">
         <v>4</v>
       </c>
@@ -9977,7 +9977,7 @@
         <v>42084</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="140">
         <v>7</v>
       </c>
@@ -10104,7 +10104,7 @@
         <v>42105</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="140">
         <v>10</v>
       </c>
@@ -10148,7 +10148,7 @@
         <v>11856250</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="140">
         <v>11</v>
       </c>
@@ -10346,7 +10346,7 @@
       <c r="M20" s="176"/>
       <c r="N20" s="176"/>
     </row>
-    <row r="21" spans="1:15" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="171"/>
       <c r="B21" s="172"/>
       <c r="C21" s="171"/>
@@ -10388,7 +10388,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="171"/>
       <c r="B23" s="172"/>
       <c r="C23" s="171"/>
@@ -10409,7 +10409,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="171"/>
       <c r="B24" s="172"/>
       <c r="C24" s="171"/>
@@ -10430,7 +10430,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="171"/>
       <c r="B25" s="172"/>
       <c r="C25" s="171"/>
@@ -10611,7 +10611,7 @@
       <c r="M35" s="176"/>
       <c r="N35" s="176"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="171"/>
       <c r="B36" s="171"/>
       <c r="C36" s="171"/>
@@ -10627,7 +10627,7 @@
       <c r="M36" s="176"/>
       <c r="N36" s="176"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="171"/>
       <c r="B37" s="171"/>
       <c r="C37" s="171"/>
@@ -10643,7 +10643,7 @@
       <c r="M37" s="176"/>
       <c r="N37" s="176"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="171"/>
       <c r="B38" s="171"/>
       <c r="C38" s="171"/>
@@ -10659,7 +10659,7 @@
       <c r="M38" s="176"/>
       <c r="N38" s="176"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="171"/>
       <c r="B39" s="171"/>
       <c r="C39" s="171"/>
@@ -10675,7 +10675,7 @@
       <c r="M39" s="176"/>
       <c r="N39" s="176"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="171"/>
       <c r="B40" s="171"/>
       <c r="C40" s="171"/>
@@ -10691,127 +10691,127 @@
       <c r="M40" s="176"/>
       <c r="N40" s="176"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="171"/>
       <c r="N41" s="176"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="171"/>
       <c r="N42" s="176"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="171"/>
       <c r="N43" s="176"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="171"/>
       <c r="N44" s="176"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="171"/>
       <c r="N45" s="176"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="171"/>
       <c r="N46" s="176"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="171"/>
       <c r="N47" s="176"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="171"/>
       <c r="N48" s="176"/>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="171"/>
       <c r="N49" s="176"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="171"/>
       <c r="N50" s="176"/>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="171"/>
       <c r="N51" s="176"/>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="171"/>
       <c r="N52" s="176"/>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="171"/>
       <c r="N53" s="176"/>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="171"/>
       <c r="N54" s="176"/>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="171"/>
       <c r="N55" s="176"/>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="171"/>
       <c r="N56" s="176"/>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="171"/>
       <c r="N57" s="176"/>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="171"/>
       <c r="N58" s="176"/>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="171"/>
       <c r="N59" s="176"/>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="171"/>
       <c r="N60" s="176"/>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="171"/>
       <c r="N61" s="176"/>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="171"/>
       <c r="N62" s="176"/>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="171"/>
       <c r="N63" s="176"/>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="171"/>
       <c r="N64" s="176"/>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="171"/>
       <c r="N65" s="176"/>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="171"/>
       <c r="N66" s="176"/>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="171"/>
       <c r="N67" s="176"/>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="171"/>
       <c r="N68" s="176"/>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="171"/>
       <c r="N69" s="176"/>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="171"/>
       <c r="N70" s="176"/>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="171"/>
       <c r="N71" s="176"/>
     </row>

</xml_diff>